<commit_message>
Actualizacion documentos gantt, requerimientos, EDT, acta
</commit_message>
<xml_diff>
--- a/FASE1/DOCS/EVIDENCIAS_GRUPALES/ENTREGABLES/Matriz EDT.xlsx
+++ b/FASE1/DOCS/EVIDENCIAS_GRUPALES/ENTREGABLES/Matriz EDT.xlsx
@@ -10,14 +10,14 @@
   <calcPr/>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion2">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId6" roundtripDataChecksum="e2eDcWhzngbnW0hzUct0N164RCqL6lYwzen7IZlyk+I="/>
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId6" roundtripDataChecksum="LeARRrPx/uazhj5IN+gtJBd9W6McP4tE1kMCkYT5Srg="/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="226" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="246" uniqueCount="130">
   <si>
     <t>Matriz Estructura de descomposición de tareas EDT</t>
   </si>
@@ -34,6 +34,9 @@
     <t>DICCIONARIO EDT</t>
   </si>
   <si>
+    <t>columna con valores de tarea</t>
+  </si>
+  <si>
     <t>Fase de Planificación</t>
   </si>
   <si>
@@ -61,39 +64,84 @@
     <t>NOMBRE ACTOR</t>
   </si>
   <si>
+    <t>CALCULOS SUELDO</t>
+  </si>
+  <si>
     <t>Acta de Constitución de proyecto</t>
   </si>
   <si>
     <t>S1</t>
   </si>
   <si>
+    <t xml:space="preserve">Jefe de Proyecto </t>
+  </si>
+  <si>
+    <t>Matias Acuna -</t>
+  </si>
+  <si>
+    <t>Sueldo diario = $68.182</t>
+  </si>
+  <si>
+    <t>$1.500.000</t>
+  </si>
+  <si>
+    <t>$600.000</t>
+  </si>
+  <si>
+    <t>Organización del equipo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">S1 </t>
+  </si>
+  <si>
+    <t>Fabian Carrasco</t>
+  </si>
+  <si>
+    <t>Valor hora (8hr) = $8.523</t>
+  </si>
+  <si>
+    <t>$1.500.001</t>
+  </si>
+  <si>
+    <t>$750.000</t>
+  </si>
+  <si>
+    <t>Definición de requerimientos Generales</t>
+  </si>
+  <si>
+    <t>S2</t>
+  </si>
+  <si>
     <t>Matias Acuna</t>
   </si>
   <si>
-    <t>Organización del equipo</t>
-  </si>
-  <si>
-    <t xml:space="preserve">S1 </t>
-  </si>
-  <si>
-    <t>Fabian Carrasco</t>
-  </si>
-  <si>
-    <t>Definición de requerimientos Generales</t>
-  </si>
-  <si>
-    <t>S2</t>
+    <t>Valor hora (9hr) = $7.526</t>
+  </si>
+  <si>
+    <t>$1.500.002</t>
   </si>
   <si>
     <t>Aprobación acta de constitución</t>
   </si>
   <si>
+    <t>$1.500.003</t>
+  </si>
+  <si>
+    <t>$150.000</t>
+  </si>
+  <si>
+    <t>$1.500.004</t>
+  </si>
+  <si>
     <t>Fase de Análisis y diseño</t>
   </si>
   <si>
     <t>Constanza Munoz</t>
   </si>
   <si>
+    <t>$1.500.005</t>
+  </si>
+  <si>
     <t xml:space="preserve">Captura de requerimientos específicos </t>
   </si>
   <si>
@@ -124,6 +172,9 @@
     <t>S5 - S6</t>
   </si>
   <si>
+    <t>abarcar sueldos</t>
+  </si>
+  <si>
     <t>Propuesta ERS</t>
   </si>
   <si>
@@ -145,22 +196,34 @@
     <t>S7 - S8</t>
   </si>
   <si>
-    <t>Mantenedores BackOffice (8 módulos)</t>
-  </si>
-  <si>
-    <t>S8 - S9</t>
-  </si>
-  <si>
-    <t>Catálogo y Carrito (Front Tienda)</t>
-  </si>
-  <si>
-    <t>S9 -S10</t>
-  </si>
-  <si>
-    <t>Autenticación y Roles</t>
-  </si>
-  <si>
-    <t>S10</t>
+    <t>Desarrollo sistema de registro de usuarios</t>
+  </si>
+  <si>
+    <t>Desarrollo sistem de autenticacion y roles</t>
+  </si>
+  <si>
+    <t>Desarrollo Catalogo de productos filtrables</t>
+  </si>
+  <si>
+    <t>Desarrollo flujo carro de compras</t>
+  </si>
+  <si>
+    <t>Desarrollo de sistema de pedidos y seguimiento</t>
+  </si>
+  <si>
+    <t>Desarrollo BackOffice sistema de registro de usuarios</t>
+  </si>
+  <si>
+    <t>Desarrollo BackOffice sistema de autenticacion y roles</t>
+  </si>
+  <si>
+    <t>Desarrollo BackOffice catalogo de productos filtrables</t>
+  </si>
+  <si>
+    <t>Desarrollo BackOffice flujo carro de compras</t>
+  </si>
+  <si>
+    <t>Desarrollo BackOffice sistema de pedidos y seguimiento</t>
   </si>
   <si>
     <t>Notificaciones por correo (registro, compra, estado pedido)</t>
@@ -373,14 +436,14 @@
       <name val="Calibri"/>
     </font>
     <font>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11.0"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
-    </font>
-    <font>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <scheme val="minor"/>
     </font>
     <font>
       <b/>
@@ -541,7 +604,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="41">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -562,6 +625,12 @@
     <xf borderId="4" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
     <xf borderId="8" fillId="3" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFill="1" applyFont="1"/>
     <xf borderId="4" fillId="3" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="4" fillId="3" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
@@ -573,30 +642,42 @@
     <xf borderId="4" fillId="3" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf borderId="9" fillId="4" fontId="4" numFmtId="0" xfId="0" applyBorder="1" applyFill="1" applyFont="1"/>
+    <xf borderId="4" fillId="3" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="3" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf borderId="9" fillId="4" fontId="5" numFmtId="0" xfId="0" applyBorder="1" applyFill="1" applyFont="1"/>
     <xf borderId="4" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="4" fillId="0" fontId="3" numFmtId="9" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" readingOrder="0"/>
     </xf>
-    <xf borderId="9" fillId="4" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="9" fillId="4" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="4" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
     </xf>
-    <xf borderId="10" fillId="4" fontId="4" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="4" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
+    </xf>
+    <xf borderId="10" fillId="4" fontId="5" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="4" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="4" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
+    <xf borderId="5" fillId="4" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0"/>
     </xf>
     <xf borderId="4" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
     </xf>
-    <xf borderId="9" fillId="4" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="9" fillId="4" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="left"/>
     </xf>
     <xf borderId="4" fillId="0" fontId="3" numFmtId="9" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
@@ -844,8 +925,8 @@
     <col customWidth="1" min="7" max="8" width="12.0"/>
     <col customWidth="1" min="9" max="9" width="5.0"/>
     <col customWidth="1" min="10" max="10" width="23.29"/>
-    <col customWidth="1" min="11" max="11" width="31.57"/>
-    <col customWidth="1" min="12" max="27" width="10.71"/>
+    <col customWidth="1" min="11" max="13" width="31.57"/>
+    <col customWidth="1" min="14" max="29" width="10.71"/>
   </cols>
   <sheetData>
     <row r="1" ht="14.25" customHeight="1"/>
@@ -877,139 +958,183 @@
         <v>4</v>
       </c>
       <c r="K4" s="8"/>
+      <c r="L4" s="9"/>
+      <c r="M4" s="10"/>
+      <c r="P4" s="11" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="5" ht="14.25" customHeight="1">
-      <c r="A5" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="B5" s="11"/>
-      <c r="C5" s="12" t="s">
+      <c r="A5" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="D5" s="12" t="s">
+      <c r="B5" s="13"/>
+      <c r="C5" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="E5" s="12" t="s">
+      <c r="D5" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="F5" s="12" t="s">
+      <c r="E5" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="G5" s="12" t="s">
+      <c r="F5" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="H5" s="13" t="s">
+      <c r="G5" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="J5" s="14" t="s">
+      <c r="H5" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="K5" s="14" t="s">
+      <c r="J5" s="16" t="s">
         <v>13</v>
       </c>
+      <c r="K5" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="L5" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="M5" s="18"/>
     </row>
     <row r="6" ht="14.25" customHeight="1" outlineLevel="1">
-      <c r="A6" s="15" t="s">
-        <v>14</v>
-      </c>
-      <c r="B6" s="16" t="s">
-        <v>15</v>
-      </c>
-      <c r="C6" s="17">
+      <c r="A6" s="19" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="C6" s="21">
         <v>0.4</v>
       </c>
-      <c r="D6" s="17">
+      <c r="D6" s="21">
         <v>0.5</v>
       </c>
       <c r="E6" s="9"/>
-      <c r="F6" s="17">
+      <c r="F6" s="21">
         <v>0.1</v>
       </c>
       <c r="G6" s="9"/>
       <c r="H6" s="5"/>
-      <c r="J6" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="K6" s="16" t="s">
-        <v>16</v>
+      <c r="J6" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="K6" s="20" t="s">
+        <v>19</v>
+      </c>
+      <c r="L6" s="20" t="s">
+        <v>20</v>
+      </c>
+      <c r="M6" s="22"/>
+      <c r="N6" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="O6" s="11" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="7" ht="14.25" customHeight="1" outlineLevel="1">
-      <c r="A7" s="18" t="s">
-        <v>17</v>
-      </c>
-      <c r="B7" s="16" t="s">
-        <v>18</v>
-      </c>
-      <c r="C7" s="17">
+      <c r="A7" s="23" t="s">
+        <v>23</v>
+      </c>
+      <c r="B7" s="20" t="s">
+        <v>24</v>
+      </c>
+      <c r="C7" s="21">
         <v>0.4</v>
       </c>
-      <c r="D7" s="17">
+      <c r="D7" s="21">
         <v>0.5</v>
       </c>
       <c r="E7" s="9"/>
-      <c r="F7" s="17">
+      <c r="F7" s="21">
         <v>0.1</v>
       </c>
       <c r="G7" s="9"/>
       <c r="H7" s="5"/>
       <c r="J7" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="K7" s="19" t="s">
-        <v>19</v>
+        <v>8</v>
+      </c>
+      <c r="K7" s="24" t="s">
+        <v>25</v>
+      </c>
+      <c r="L7" s="24" t="s">
+        <v>26</v>
+      </c>
+      <c r="M7" s="25"/>
+      <c r="N7" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="O7" s="11" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="8" ht="14.25" customHeight="1" outlineLevel="1">
-      <c r="A8" s="15" t="s">
-        <v>20</v>
-      </c>
-      <c r="B8" s="16" t="s">
-        <v>21</v>
-      </c>
-      <c r="C8" s="17">
+      <c r="A8" s="19" t="s">
+        <v>29</v>
+      </c>
+      <c r="B8" s="20" t="s">
+        <v>30</v>
+      </c>
+      <c r="C8" s="21">
         <v>0.4</v>
       </c>
-      <c r="D8" s="17">
+      <c r="D8" s="21">
         <v>0.5</v>
       </c>
       <c r="E8" s="9"/>
-      <c r="F8" s="17">
+      <c r="F8" s="21">
         <v>0.1</v>
       </c>
       <c r="G8" s="9"/>
       <c r="H8" s="5"/>
       <c r="J8" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="K8" s="16" t="s">
-        <v>16</v>
+        <v>9</v>
+      </c>
+      <c r="K8" s="20" t="s">
+        <v>31</v>
+      </c>
+      <c r="L8" s="20" t="s">
+        <v>32</v>
+      </c>
+      <c r="M8" s="22"/>
+      <c r="N8" s="11" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="9" ht="14.25" customHeight="1" outlineLevel="1">
-      <c r="A9" s="18" t="s">
-        <v>22</v>
-      </c>
-      <c r="B9" s="16" t="s">
-        <v>21</v>
-      </c>
-      <c r="C9" s="17">
+      <c r="A9" s="23" t="s">
+        <v>34</v>
+      </c>
+      <c r="B9" s="20" t="s">
+        <v>30</v>
+      </c>
+      <c r="C9" s="21">
         <v>0.4</v>
       </c>
-      <c r="D9" s="17">
+      <c r="D9" s="21">
         <v>0.5</v>
       </c>
       <c r="E9" s="9"/>
-      <c r="F9" s="17">
+      <c r="F9" s="21">
         <v>0.1</v>
       </c>
       <c r="G9" s="9"/>
       <c r="H9" s="5"/>
       <c r="J9" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="K9" s="16" t="s">
-        <v>19</v>
+        <v>10</v>
+      </c>
+      <c r="K9" s="20" t="s">
+        <v>25</v>
+      </c>
+      <c r="L9" s="20"/>
+      <c r="M9" s="22"/>
+      <c r="N9" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="O9" s="11" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="10" ht="14.25" customHeight="1" outlineLevel="1">
@@ -1022,145 +1147,163 @@
       <c r="G10" s="9"/>
       <c r="H10" s="9"/>
       <c r="J10" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="K10" s="20" t="s">
+        <v>31</v>
+      </c>
+      <c r="L10" s="20"/>
+      <c r="M10" s="22"/>
+      <c r="N10" s="11" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="11" ht="14.25" customHeight="1">
+      <c r="A11" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="B11" s="13"/>
+      <c r="C11" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="D11" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="E11" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="F11" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="K10" s="16" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="11" ht="14.25" customHeight="1">
-      <c r="A11" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="B11" s="11"/>
-      <c r="C11" s="12" t="s">
-        <v>6</v>
-      </c>
-      <c r="D11" s="12" t="s">
-        <v>7</v>
-      </c>
-      <c r="E11" s="12" t="s">
-        <v>8</v>
-      </c>
-      <c r="F11" s="12" t="s">
-        <v>9</v>
-      </c>
-      <c r="G11" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="H11" s="13" t="s">
+      <c r="G11" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="J11" s="16" t="s">
-        <v>11</v>
-      </c>
-      <c r="K11" s="16" t="s">
-        <v>24</v>
+      <c r="H11" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="J11" s="20" t="s">
+        <v>12</v>
+      </c>
+      <c r="K11" s="20" t="s">
+        <v>39</v>
+      </c>
+      <c r="L11" s="20"/>
+      <c r="M11" s="22"/>
+      <c r="N11" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="O11" s="11" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="12" ht="14.25" customHeight="1" outlineLevel="1">
-      <c r="A12" s="15" t="s">
-        <v>25</v>
-      </c>
-      <c r="B12" s="16" t="s">
-        <v>26</v>
-      </c>
-      <c r="C12" s="17">
+      <c r="A12" s="19" t="s">
+        <v>41</v>
+      </c>
+      <c r="B12" s="20" t="s">
+        <v>42</v>
+      </c>
+      <c r="C12" s="21">
         <v>0.35</v>
       </c>
-      <c r="D12" s="17"/>
+      <c r="D12" s="21"/>
       <c r="E12" s="9"/>
-      <c r="F12" s="17">
+      <c r="F12" s="21">
         <v>0.2</v>
       </c>
       <c r="G12" s="9"/>
-      <c r="H12" s="17">
+      <c r="H12" s="21">
         <v>0.45</v>
       </c>
     </row>
     <row r="13" ht="14.25" customHeight="1" outlineLevel="1">
-      <c r="A13" s="20" t="s">
-        <v>27</v>
-      </c>
-      <c r="B13" s="16" t="s">
-        <v>28</v>
-      </c>
-      <c r="C13" s="17">
+      <c r="A13" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="B13" s="20" t="s">
+        <v>44</v>
+      </c>
+      <c r="C13" s="21">
         <v>0.6</v>
       </c>
-      <c r="D13" s="17">
+      <c r="D13" s="21">
         <v>0.15</v>
       </c>
       <c r="E13" s="9"/>
-      <c r="F13" s="17">
+      <c r="F13" s="21">
         <v>0.25</v>
       </c>
       <c r="G13" s="9"/>
-      <c r="H13" s="17"/>
-      <c r="J13" s="21" t="s">
-        <v>29</v>
-      </c>
-      <c r="K13" s="21" t="s">
-        <v>30</v>
-      </c>
+      <c r="H13" s="21"/>
+      <c r="J13" s="27" t="s">
+        <v>45</v>
+      </c>
+      <c r="K13" s="27" t="s">
+        <v>46</v>
+      </c>
+      <c r="L13" s="11"/>
+      <c r="M13" s="11"/>
     </row>
     <row r="14" ht="14.25" customHeight="1" outlineLevel="1">
-      <c r="A14" s="15" t="s">
-        <v>31</v>
-      </c>
-      <c r="B14" s="16" t="s">
-        <v>32</v>
-      </c>
-      <c r="C14" s="17">
+      <c r="A14" s="19" t="s">
+        <v>47</v>
+      </c>
+      <c r="B14" s="20" t="s">
+        <v>48</v>
+      </c>
+      <c r="C14" s="21">
         <v>0.35</v>
       </c>
       <c r="D14" s="9"/>
       <c r="E14" s="9"/>
-      <c r="F14" s="17">
+      <c r="F14" s="21">
         <v>0.2</v>
       </c>
       <c r="G14" s="9"/>
-      <c r="H14" s="17">
+      <c r="H14" s="21">
         <v>0.45</v>
       </c>
     </row>
     <row r="15" ht="14.25" customHeight="1" outlineLevel="1">
-      <c r="A15" s="15" t="s">
-        <v>33</v>
-      </c>
-      <c r="B15" s="16" t="s">
-        <v>34</v>
-      </c>
-      <c r="C15" s="17">
+      <c r="A15" s="19" t="s">
+        <v>49</v>
+      </c>
+      <c r="B15" s="20" t="s">
+        <v>50</v>
+      </c>
+      <c r="C15" s="21">
         <v>0.3</v>
       </c>
       <c r="D15" s="5"/>
       <c r="E15" s="9"/>
-      <c r="F15" s="17">
+      <c r="F15" s="21">
         <v>0.2</v>
       </c>
-      <c r="G15" s="17">
+      <c r="G15" s="21">
         <v>0.5</v>
       </c>
-      <c r="H15" s="17"/>
+      <c r="H15" s="21"/>
+      <c r="J15" s="11" t="s">
+        <v>51</v>
+      </c>
     </row>
     <row r="16" ht="14.25" customHeight="1" outlineLevel="1">
-      <c r="A16" s="15" t="s">
-        <v>35</v>
-      </c>
-      <c r="B16" s="16" t="s">
-        <v>36</v>
-      </c>
-      <c r="C16" s="17">
+      <c r="A16" s="19" t="s">
+        <v>52</v>
+      </c>
+      <c r="B16" s="20" t="s">
+        <v>53</v>
+      </c>
+      <c r="C16" s="21">
         <v>0.35</v>
       </c>
       <c r="D16" s="9"/>
       <c r="E16" s="9"/>
-      <c r="F16" s="17">
+      <c r="F16" s="21">
         <v>0.2</v>
       </c>
       <c r="G16" s="9"/>
-      <c r="H16" s="17">
+      <c r="H16" s="21">
         <v>0.45</v>
       </c>
     </row>
@@ -1175,402 +1318,322 @@
       <c r="H17" s="9"/>
     </row>
     <row r="18" ht="14.25" customHeight="1">
-      <c r="A18" s="11" t="s">
-        <v>37</v>
-      </c>
-      <c r="B18" s="11"/>
-      <c r="C18" s="12" t="s">
-        <v>6</v>
-      </c>
-      <c r="D18" s="12" t="s">
+      <c r="A18" s="13" t="s">
+        <v>54</v>
+      </c>
+      <c r="B18" s="13"/>
+      <c r="C18" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="E18" s="12" t="s">
+      <c r="D18" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="F18" s="12" t="s">
+      <c r="E18" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="G18" s="12" t="s">
+      <c r="F18" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="H18" s="13" t="s">
+      <c r="G18" s="14" t="s">
         <v>11</v>
       </c>
+      <c r="H18" s="15" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="19" ht="18.0" customHeight="1" outlineLevel="1">
-      <c r="A19" s="15" t="s">
-        <v>38</v>
-      </c>
-      <c r="B19" s="16" t="s">
-        <v>39</v>
-      </c>
-      <c r="C19" s="17">
+      <c r="A19" s="19" t="s">
+        <v>55</v>
+      </c>
+      <c r="B19" s="20" t="s">
+        <v>56</v>
+      </c>
+      <c r="C19" s="21">
         <v>0.2</v>
       </c>
-      <c r="D19" s="17">
+      <c r="D19" s="21">
         <v>0.6</v>
       </c>
-      <c r="E19" s="17">
+      <c r="E19" s="21">
         <v>0.05</v>
       </c>
-      <c r="F19" s="17">
+      <c r="F19" s="21">
         <v>0.15</v>
       </c>
       <c r="G19" s="9"/>
       <c r="H19" s="5"/>
     </row>
     <row r="20" ht="18.0" customHeight="1" outlineLevel="1">
-      <c r="A20" s="18" t="s">
-        <v>40</v>
-      </c>
-      <c r="B20" s="16" t="s">
-        <v>41</v>
-      </c>
-      <c r="C20" s="17">
+      <c r="A20" s="23" t="s">
+        <v>57</v>
+      </c>
+      <c r="B20" s="20" t="s">
+        <v>58</v>
+      </c>
+      <c r="C20" s="21">
         <v>0.1</v>
       </c>
-      <c r="D20" s="17">
+      <c r="D20" s="21">
         <v>0.4</v>
       </c>
-      <c r="E20" s="17">
+      <c r="E20" s="21">
         <v>0.4</v>
       </c>
-      <c r="F20" s="17">
+      <c r="F20" s="21">
         <v>0.1</v>
       </c>
       <c r="G20" s="9"/>
       <c r="H20" s="9"/>
     </row>
     <row r="21" ht="18.0" customHeight="1" outlineLevel="1">
-      <c r="A21" s="18" t="s">
-        <v>42</v>
-      </c>
-      <c r="B21" s="16" t="s">
-        <v>43</v>
-      </c>
-      <c r="C21" s="17">
-        <v>0.2</v>
-      </c>
-      <c r="D21" s="17">
-        <v>0.6</v>
-      </c>
-      <c r="E21" s="17">
-        <v>0.05</v>
-      </c>
-      <c r="F21" s="17">
-        <v>0.15</v>
-      </c>
+      <c r="A21" s="23" t="s">
+        <v>59</v>
+      </c>
+      <c r="B21" s="20"/>
+      <c r="C21" s="21"/>
+      <c r="D21" s="21"/>
+      <c r="E21" s="21"/>
+      <c r="F21" s="21"/>
       <c r="G21" s="9"/>
-      <c r="H21" s="5"/>
+      <c r="H21" s="9"/>
     </row>
     <row r="22" ht="18.0" customHeight="1" outlineLevel="1">
-      <c r="A22" s="22" t="s">
-        <v>44</v>
-      </c>
-      <c r="B22" s="16" t="s">
-        <v>45</v>
-      </c>
-      <c r="C22" s="17">
-        <v>0.2</v>
-      </c>
-      <c r="D22" s="17">
-        <v>0.6</v>
-      </c>
-      <c r="E22" s="17">
-        <v>0.05</v>
-      </c>
-      <c r="F22" s="17">
-        <v>0.15</v>
-      </c>
+      <c r="A22" s="23" t="s">
+        <v>60</v>
+      </c>
+      <c r="B22" s="20"/>
+      <c r="C22" s="21"/>
+      <c r="D22" s="21"/>
+      <c r="E22" s="21"/>
+      <c r="F22" s="21"/>
       <c r="G22" s="9"/>
-      <c r="H22" s="5"/>
+      <c r="H22" s="9"/>
     </row>
     <row r="23" ht="18.0" customHeight="1" outlineLevel="1">
       <c r="A23" s="23" t="s">
-        <v>46</v>
-      </c>
-      <c r="B23" s="16" t="s">
-        <v>47</v>
-      </c>
-      <c r="C23" s="17">
-        <v>0.2</v>
-      </c>
-      <c r="D23" s="17">
-        <v>0.6</v>
-      </c>
-      <c r="E23" s="17">
-        <v>0.05</v>
-      </c>
-      <c r="F23" s="17">
-        <v>0.15</v>
-      </c>
+        <v>61</v>
+      </c>
+      <c r="B23" s="20"/>
+      <c r="C23" s="21"/>
+      <c r="D23" s="21"/>
+      <c r="E23" s="21"/>
+      <c r="F23" s="21"/>
       <c r="G23" s="9"/>
-      <c r="H23" s="5"/>
-    </row>
-    <row r="24" ht="27.75" customHeight="1" outlineLevel="1">
+      <c r="H23" s="9"/>
+    </row>
+    <row r="24" ht="18.0" customHeight="1" outlineLevel="1">
       <c r="A24" s="23" t="s">
-        <v>48</v>
-      </c>
-      <c r="B24" s="16" t="s">
-        <v>49</v>
-      </c>
-      <c r="C24" s="17">
-        <v>0.2</v>
-      </c>
-      <c r="D24" s="17">
-        <v>0.6</v>
-      </c>
-      <c r="E24" s="17">
-        <v>0.05</v>
-      </c>
-      <c r="F24" s="17">
-        <v>0.15</v>
-      </c>
+        <v>62</v>
+      </c>
+      <c r="B24" s="20"/>
+      <c r="C24" s="21"/>
+      <c r="D24" s="21"/>
+      <c r="E24" s="21"/>
+      <c r="F24" s="21"/>
       <c r="G24" s="9"/>
-      <c r="H24" s="5"/>
+      <c r="H24" s="9"/>
     </row>
     <row r="25" ht="18.0" customHeight="1" outlineLevel="1">
       <c r="A25" s="23" t="s">
-        <v>50</v>
-      </c>
-      <c r="B25" s="16" t="s">
-        <v>51</v>
-      </c>
-      <c r="C25" s="17">
+        <v>63</v>
+      </c>
+      <c r="B25" s="20"/>
+      <c r="C25" s="21"/>
+      <c r="D25" s="21"/>
+      <c r="E25" s="21"/>
+      <c r="F25" s="21"/>
+      <c r="G25" s="9"/>
+      <c r="H25" s="9"/>
+    </row>
+    <row r="26" ht="18.0" customHeight="1" outlineLevel="1">
+      <c r="A26" s="28" t="s">
+        <v>64</v>
+      </c>
+      <c r="B26" s="20"/>
+      <c r="C26" s="21"/>
+      <c r="D26" s="21"/>
+      <c r="E26" s="21"/>
+      <c r="F26" s="21"/>
+      <c r="G26" s="9"/>
+      <c r="H26" s="5"/>
+    </row>
+    <row r="27" ht="18.0" customHeight="1" outlineLevel="1">
+      <c r="A27" s="28" t="s">
+        <v>65</v>
+      </c>
+      <c r="B27" s="20"/>
+      <c r="C27" s="21"/>
+      <c r="D27" s="21"/>
+      <c r="E27" s="21"/>
+      <c r="F27" s="21"/>
+      <c r="G27" s="9"/>
+      <c r="H27" s="5"/>
+    </row>
+    <row r="28" ht="18.0" customHeight="1" outlineLevel="1">
+      <c r="A28" s="28" t="s">
+        <v>66</v>
+      </c>
+      <c r="B28" s="20"/>
+      <c r="C28" s="21"/>
+      <c r="D28" s="21"/>
+      <c r="E28" s="21"/>
+      <c r="F28" s="21"/>
+      <c r="G28" s="9"/>
+      <c r="H28" s="5"/>
+    </row>
+    <row r="29" ht="18.0" customHeight="1" outlineLevel="1">
+      <c r="A29" s="28" t="s">
+        <v>67</v>
+      </c>
+      <c r="B29" s="20"/>
+      <c r="C29" s="21"/>
+      <c r="D29" s="21"/>
+      <c r="E29" s="21"/>
+      <c r="F29" s="21"/>
+      <c r="G29" s="9"/>
+      <c r="H29" s="5"/>
+    </row>
+    <row r="30" ht="18.0" customHeight="1" outlineLevel="1">
+      <c r="A30" s="28" t="s">
+        <v>68</v>
+      </c>
+      <c r="B30" s="20"/>
+      <c r="C30" s="21"/>
+      <c r="D30" s="21"/>
+      <c r="E30" s="21"/>
+      <c r="F30" s="21"/>
+      <c r="G30" s="9"/>
+      <c r="H30" s="5"/>
+    </row>
+    <row r="31" ht="27.75" customHeight="1" outlineLevel="1">
+      <c r="A31" s="29" t="s">
+        <v>69</v>
+      </c>
+      <c r="B31" s="20" t="s">
+        <v>70</v>
+      </c>
+      <c r="C31" s="21">
         <v>0.2</v>
       </c>
-      <c r="D25" s="17">
+      <c r="D31" s="21">
         <v>0.6</v>
       </c>
-      <c r="E25" s="17">
+      <c r="E31" s="21">
         <v>0.05</v>
       </c>
-      <c r="F25" s="17">
+      <c r="F31" s="21">
         <v>0.15</v>
       </c>
-      <c r="G25" s="9"/>
-      <c r="H25" s="5"/>
-    </row>
-    <row r="26" ht="14.25" customHeight="1">
-      <c r="A26" s="11" t="s">
-        <v>52</v>
-      </c>
-      <c r="B26" s="11"/>
-      <c r="C26" s="12" t="s">
-        <v>6</v>
-      </c>
-      <c r="D26" s="12" t="s">
+      <c r="G31" s="9"/>
+      <c r="H31" s="5"/>
+    </row>
+    <row r="32" ht="18.0" customHeight="1" outlineLevel="1">
+      <c r="A32" s="29" t="s">
+        <v>71</v>
+      </c>
+      <c r="B32" s="20" t="s">
+        <v>72</v>
+      </c>
+      <c r="C32" s="21">
+        <v>0.2</v>
+      </c>
+      <c r="D32" s="21">
+        <v>0.6</v>
+      </c>
+      <c r="E32" s="21">
+        <v>0.05</v>
+      </c>
+      <c r="F32" s="21">
+        <v>0.15</v>
+      </c>
+      <c r="G32" s="9"/>
+      <c r="H32" s="5"/>
+    </row>
+    <row r="33" ht="14.25" customHeight="1">
+      <c r="A33" s="13" t="s">
+        <v>73</v>
+      </c>
+      <c r="B33" s="13"/>
+      <c r="C33" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="E26" s="12" t="s">
+      <c r="D33" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="F26" s="12" t="s">
+      <c r="E33" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="G26" s="12" t="s">
+      <c r="F33" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="H26" s="13" t="s">
+      <c r="G33" s="14" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="27" ht="14.25" customHeight="1">
-      <c r="A27" s="24" t="s">
-        <v>53</v>
-      </c>
-      <c r="B27" s="16" t="s">
-        <v>54</v>
-      </c>
-      <c r="C27" s="25">
+      <c r="H33" s="15" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="34" ht="14.25" customHeight="1">
+      <c r="A34" s="30" t="s">
+        <v>74</v>
+      </c>
+      <c r="B34" s="20" t="s">
+        <v>75</v>
+      </c>
+      <c r="C34" s="31">
         <v>0.15</v>
       </c>
-      <c r="D27" s="4"/>
-      <c r="E27" s="4"/>
-      <c r="F27" s="25">
-        <v>0.7</v>
-      </c>
-      <c r="G27" s="4"/>
-      <c r="H27" s="25">
-        <v>0.15</v>
-      </c>
-    </row>
-    <row r="28" ht="14.25" customHeight="1" outlineLevel="1">
-      <c r="A28" s="24" t="s">
-        <v>55</v>
-      </c>
-      <c r="B28" s="16" t="s">
-        <v>56</v>
-      </c>
-      <c r="C28" s="25">
-        <v>0.15</v>
-      </c>
-      <c r="D28" s="16"/>
-      <c r="E28" s="4"/>
-      <c r="F28" s="25">
-        <v>0.7</v>
-      </c>
-      <c r="G28" s="4"/>
-      <c r="H28" s="25">
-        <v>0.15</v>
-      </c>
-    </row>
-    <row r="29" ht="14.25" customHeight="1" outlineLevel="1">
-      <c r="A29" s="24" t="s">
-        <v>57</v>
-      </c>
-      <c r="B29" s="16" t="s">
-        <v>58</v>
-      </c>
-      <c r="C29" s="25">
-        <v>0.15</v>
-      </c>
-      <c r="D29" s="4"/>
-      <c r="E29" s="4"/>
-      <c r="F29" s="25">
-        <v>0.7</v>
-      </c>
-      <c r="G29" s="4"/>
-      <c r="H29" s="25">
-        <v>0.15</v>
-      </c>
-    </row>
-    <row r="30" ht="14.25" customHeight="1" outlineLevel="1">
-      <c r="A30" s="4"/>
-      <c r="B30" s="4"/>
-      <c r="C30" s="4"/>
-      <c r="D30" s="4"/>
-      <c r="E30" s="4"/>
-      <c r="F30" s="4"/>
-      <c r="G30" s="4"/>
-      <c r="H30" s="4"/>
-    </row>
-    <row r="31" ht="14.25" customHeight="1" outlineLevel="1">
-      <c r="A31" s="11" t="s">
-        <v>59</v>
-      </c>
-      <c r="B31" s="11"/>
-      <c r="C31" s="12" t="s">
-        <v>6</v>
-      </c>
-      <c r="D31" s="12" t="s">
-        <v>7</v>
-      </c>
-      <c r="E31" s="12" t="s">
-        <v>8</v>
-      </c>
-      <c r="F31" s="12" t="s">
-        <v>9</v>
-      </c>
-      <c r="G31" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="H31" s="13" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="32" ht="14.25" customHeight="1">
-      <c r="A32" s="24" t="s">
-        <v>60</v>
-      </c>
-      <c r="B32" s="16" t="s">
-        <v>61</v>
-      </c>
-      <c r="C32" s="25">
-        <v>0.3</v>
-      </c>
-      <c r="D32" s="25">
-        <v>0.5</v>
-      </c>
-      <c r="E32" s="4"/>
-      <c r="F32" s="25">
-        <v>0.2</v>
-      </c>
-      <c r="G32" s="4"/>
-      <c r="H32" s="4"/>
-    </row>
-    <row r="33" ht="14.25" customHeight="1" outlineLevel="1">
-      <c r="A33" s="24" t="s">
-        <v>62</v>
-      </c>
-      <c r="B33" s="16" t="s">
-        <v>63</v>
-      </c>
-      <c r="C33" s="4"/>
-      <c r="D33" s="4"/>
-      <c r="E33" s="4"/>
-      <c r="F33" s="25">
-        <v>0.4</v>
-      </c>
-      <c r="G33" s="4"/>
-      <c r="H33" s="25">
-        <v>0.6</v>
-      </c>
-    </row>
-    <row r="34" ht="14.25" customHeight="1" outlineLevel="1">
-      <c r="A34" s="24" t="s">
-        <v>64</v>
-      </c>
-      <c r="B34" s="16" t="s">
-        <v>65</v>
-      </c>
-      <c r="C34" s="4"/>
       <c r="D34" s="4"/>
       <c r="E34" s="4"/>
-      <c r="F34" s="25">
-        <v>0.4</v>
+      <c r="F34" s="31">
+        <v>0.7</v>
       </c>
       <c r="G34" s="4"/>
-      <c r="H34" s="25">
-        <v>0.6</v>
+      <c r="H34" s="31">
+        <v>0.15</v>
       </c>
     </row>
     <row r="35" ht="14.25" customHeight="1" outlineLevel="1">
-      <c r="A35" s="24" t="s">
-        <v>66</v>
-      </c>
-      <c r="B35" s="16" t="s">
-        <v>67</v>
-      </c>
-      <c r="C35" s="25">
-        <v>0.4</v>
-      </c>
-      <c r="D35" s="4"/>
+      <c r="A35" s="30" t="s">
+        <v>76</v>
+      </c>
+      <c r="B35" s="20" t="s">
+        <v>77</v>
+      </c>
+      <c r="C35" s="31">
+        <v>0.15</v>
+      </c>
+      <c r="D35" s="20"/>
       <c r="E35" s="4"/>
-      <c r="F35" s="25"/>
+      <c r="F35" s="31">
+        <v>0.7</v>
+      </c>
       <c r="G35" s="4"/>
-      <c r="H35" s="25">
-        <v>0.6</v>
+      <c r="H35" s="31">
+        <v>0.15</v>
       </c>
     </row>
     <row r="36" ht="14.25" customHeight="1" outlineLevel="1">
-      <c r="A36" s="16" t="s">
-        <v>68</v>
-      </c>
-      <c r="B36" s="16" t="s">
-        <v>69</v>
-      </c>
-      <c r="C36" s="25">
-        <v>1.0</v>
-      </c>
-      <c r="D36" s="25">
-        <v>1.0</v>
-      </c>
-      <c r="E36" s="25">
-        <v>1.0</v>
-      </c>
-      <c r="F36" s="25">
-        <v>1.0</v>
-      </c>
-      <c r="G36" s="25">
-        <v>1.0</v>
-      </c>
-      <c r="H36" s="25">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="37" ht="14.25" customHeight="1">
+      <c r="A36" s="30" t="s">
+        <v>78</v>
+      </c>
+      <c r="B36" s="20" t="s">
+        <v>79</v>
+      </c>
+      <c r="C36" s="31">
+        <v>0.15</v>
+      </c>
+      <c r="D36" s="4"/>
+      <c r="E36" s="4"/>
+      <c r="F36" s="31">
+        <v>0.7</v>
+      </c>
+      <c r="G36" s="4"/>
+      <c r="H36" s="31">
+        <v>0.15</v>
+      </c>
+    </row>
+    <row r="37" ht="14.25" customHeight="1" outlineLevel="1">
       <c r="A37" s="4"/>
       <c r="B37" s="4"/>
       <c r="C37" s="4"/>
@@ -1580,23 +1643,150 @@
       <c r="G37" s="4"/>
       <c r="H37" s="4"/>
     </row>
-    <row r="38" ht="14.25" customHeight="1">
-      <c r="A38" s="4"/>
-      <c r="B38" s="4"/>
-      <c r="C38" s="4"/>
-      <c r="D38" s="4"/>
-      <c r="E38" s="4"/>
-      <c r="F38" s="4"/>
-      <c r="G38" s="4"/>
-      <c r="H38" s="4"/>
-    </row>
-    <row r="39" ht="14.25" customHeight="1"/>
-    <row r="40" ht="14.25" customHeight="1"/>
-    <row r="41" ht="14.25" customHeight="1"/>
-    <row r="42" ht="14.25" customHeight="1"/>
-    <row r="43" ht="14.25" customHeight="1"/>
-    <row r="44" ht="14.25" customHeight="1"/>
-    <row r="45" ht="14.25" customHeight="1"/>
+    <row r="38" ht="14.25" customHeight="1" outlineLevel="1">
+      <c r="A38" s="13" t="s">
+        <v>80</v>
+      </c>
+      <c r="B38" s="13"/>
+      <c r="C38" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="D38" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="E38" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="F38" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="G38" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="H38" s="15" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="39" ht="14.25" customHeight="1">
+      <c r="A39" s="30" t="s">
+        <v>81</v>
+      </c>
+      <c r="B39" s="20" t="s">
+        <v>82</v>
+      </c>
+      <c r="C39" s="31">
+        <v>0.3</v>
+      </c>
+      <c r="D39" s="31">
+        <v>0.5</v>
+      </c>
+      <c r="E39" s="4"/>
+      <c r="F39" s="31">
+        <v>0.2</v>
+      </c>
+      <c r="G39" s="4"/>
+      <c r="H39" s="4"/>
+    </row>
+    <row r="40" ht="14.25" customHeight="1" outlineLevel="1">
+      <c r="A40" s="30" t="s">
+        <v>83</v>
+      </c>
+      <c r="B40" s="20" t="s">
+        <v>84</v>
+      </c>
+      <c r="C40" s="4"/>
+      <c r="D40" s="4"/>
+      <c r="E40" s="4"/>
+      <c r="F40" s="31">
+        <v>0.4</v>
+      </c>
+      <c r="G40" s="4"/>
+      <c r="H40" s="31">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="41" ht="14.25" customHeight="1" outlineLevel="1">
+      <c r="A41" s="30" t="s">
+        <v>85</v>
+      </c>
+      <c r="B41" s="20" t="s">
+        <v>86</v>
+      </c>
+      <c r="C41" s="4"/>
+      <c r="D41" s="4"/>
+      <c r="E41" s="4"/>
+      <c r="F41" s="31">
+        <v>0.4</v>
+      </c>
+      <c r="G41" s="4"/>
+      <c r="H41" s="31">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="42" ht="14.25" customHeight="1" outlineLevel="1">
+      <c r="A42" s="30" t="s">
+        <v>87</v>
+      </c>
+      <c r="B42" s="20" t="s">
+        <v>88</v>
+      </c>
+      <c r="C42" s="31">
+        <v>0.4</v>
+      </c>
+      <c r="D42" s="4"/>
+      <c r="E42" s="4"/>
+      <c r="F42" s="31"/>
+      <c r="G42" s="4"/>
+      <c r="H42" s="31">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="43" ht="14.25" customHeight="1" outlineLevel="1">
+      <c r="A43" s="20" t="s">
+        <v>89</v>
+      </c>
+      <c r="B43" s="20" t="s">
+        <v>90</v>
+      </c>
+      <c r="C43" s="31">
+        <v>1.0</v>
+      </c>
+      <c r="D43" s="31">
+        <v>1.0</v>
+      </c>
+      <c r="E43" s="31">
+        <v>1.0</v>
+      </c>
+      <c r="F43" s="31">
+        <v>1.0</v>
+      </c>
+      <c r="G43" s="31">
+        <v>1.0</v>
+      </c>
+      <c r="H43" s="31">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="44" ht="14.25" customHeight="1">
+      <c r="A44" s="4"/>
+      <c r="B44" s="4"/>
+      <c r="C44" s="4"/>
+      <c r="D44" s="4"/>
+      <c r="E44" s="4"/>
+      <c r="F44" s="4"/>
+      <c r="G44" s="4"/>
+      <c r="H44" s="4"/>
+    </row>
+    <row r="45" ht="14.25" customHeight="1">
+      <c r="A45" s="4"/>
+      <c r="B45" s="4"/>
+      <c r="C45" s="4"/>
+      <c r="D45" s="4"/>
+      <c r="E45" s="4"/>
+      <c r="F45" s="4"/>
+      <c r="G45" s="4"/>
+      <c r="H45" s="4"/>
+    </row>
     <row r="46" ht="14.25" customHeight="1"/>
     <row r="47" ht="14.25" customHeight="1"/>
     <row r="48" ht="14.25" customHeight="1"/>
@@ -2531,6 +2721,13 @@
     <row r="977" ht="14.25" customHeight="1"/>
     <row r="978" ht="14.25" customHeight="1"/>
     <row r="979" ht="14.25" customHeight="1"/>
+    <row r="980" ht="14.25" customHeight="1"/>
+    <row r="981" ht="14.25" customHeight="1"/>
+    <row r="982" ht="14.25" customHeight="1"/>
+    <row r="983" ht="14.25" customHeight="1"/>
+    <row r="984" ht="14.25" customHeight="1"/>
+    <row r="985" ht="14.25" customHeight="1"/>
+    <row r="986" ht="14.25" customHeight="1"/>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="A2:D2"/>
@@ -2570,78 +2767,78 @@
   <sheetData>
     <row r="1" ht="14.25" customHeight="1"/>
     <row r="2" ht="14.25" customHeight="1">
-      <c r="A2" s="14" t="s">
-        <v>70</v>
-      </c>
-      <c r="B2" s="14" t="s">
-        <v>71</v>
-      </c>
-      <c r="C2" s="14" t="s">
-        <v>72</v>
-      </c>
-      <c r="D2" s="12" t="s">
-        <v>73</v>
-      </c>
-      <c r="E2" s="14" t="s">
-        <v>74</v>
-      </c>
-      <c r="F2" s="14" t="s">
-        <v>75</v>
-      </c>
-      <c r="H2" s="26" t="s">
-        <v>76</v>
-      </c>
-      <c r="I2" s="27"/>
-      <c r="J2" s="27"/>
-      <c r="K2" s="28"/>
+      <c r="A2" s="16" t="s">
+        <v>91</v>
+      </c>
+      <c r="B2" s="16" t="s">
+        <v>92</v>
+      </c>
+      <c r="C2" s="16" t="s">
+        <v>93</v>
+      </c>
+      <c r="D2" s="14" t="s">
+        <v>94</v>
+      </c>
+      <c r="E2" s="16" t="s">
+        <v>95</v>
+      </c>
+      <c r="F2" s="16" t="s">
+        <v>96</v>
+      </c>
+      <c r="H2" s="32" t="s">
+        <v>97</v>
+      </c>
+      <c r="I2" s="33"/>
+      <c r="J2" s="33"/>
+      <c r="K2" s="34"/>
     </row>
     <row r="3" ht="14.25" customHeight="1">
       <c r="A3" s="4" t="s">
-        <v>77</v>
+        <v>98</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C3" s="4"/>
       <c r="D3" s="4"/>
-      <c r="E3" s="29">
+      <c r="E3" s="35">
         <v>0.0</v>
       </c>
-      <c r="F3" s="30">
+      <c r="F3" s="36">
         <f t="shared" ref="F3:F7" si="1">D3*E3</f>
         <v>0</v>
       </c>
-      <c r="H3" s="14" t="s">
-        <v>71</v>
-      </c>
-      <c r="I3" s="14" t="s">
-        <v>72</v>
-      </c>
-      <c r="J3" s="14" t="s">
-        <v>78</v>
-      </c>
-      <c r="K3" s="14" t="s">
-        <v>79</v>
+      <c r="H3" s="16" t="s">
+        <v>92</v>
+      </c>
+      <c r="I3" s="16" t="s">
+        <v>93</v>
+      </c>
+      <c r="J3" s="16" t="s">
+        <v>99</v>
+      </c>
+      <c r="K3" s="16" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="4" ht="14.25" customHeight="1">
       <c r="A4" s="4" t="s">
-        <v>80</v>
+        <v>101</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C4" s="31"/>
+        <v>8</v>
+      </c>
+      <c r="C4" s="37"/>
       <c r="D4" s="4"/>
-      <c r="E4" s="29">
+      <c r="E4" s="35">
         <v>0.0</v>
       </c>
-      <c r="F4" s="30">
+      <c r="F4" s="36">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="H4" s="4" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="I4" s="4"/>
       <c r="J4" s="4"/>
@@ -2649,45 +2846,45 @@
     </row>
     <row r="5" ht="14.25" customHeight="1">
       <c r="A5" s="4" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>81</v>
+        <v>102</v>
       </c>
       <c r="C5" s="4"/>
       <c r="D5" s="4"/>
-      <c r="E5" s="29">
+      <c r="E5" s="35">
         <v>0.0</v>
       </c>
-      <c r="F5" s="30">
+      <c r="F5" s="36">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="H5" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="I5" s="31"/>
+        <v>8</v>
+      </c>
+      <c r="I5" s="37"/>
       <c r="J5" s="4"/>
       <c r="K5" s="4"/>
     </row>
     <row r="6" ht="14.25" customHeight="1">
       <c r="A6" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>82</v>
+        <v>103</v>
       </c>
       <c r="C6" s="4"/>
       <c r="D6" s="4"/>
-      <c r="E6" s="29">
+      <c r="E6" s="35">
         <v>0.0</v>
       </c>
-      <c r="F6" s="30">
+      <c r="F6" s="36">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="H6" s="4" t="s">
-        <v>83</v>
+        <v>104</v>
       </c>
       <c r="I6" s="4"/>
       <c r="J6" s="4"/>
@@ -2695,22 +2892,22 @@
     </row>
     <row r="7" ht="14.25" customHeight="1">
       <c r="A7" s="4" t="s">
-        <v>84</v>
+        <v>105</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C7" s="4"/>
       <c r="D7" s="4"/>
-      <c r="E7" s="29">
+      <c r="E7" s="35">
         <v>0.0</v>
       </c>
-      <c r="F7" s="30">
+      <c r="F7" s="36">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="H7" s="4" t="s">
-        <v>82</v>
+        <v>103</v>
       </c>
       <c r="I7" s="4"/>
       <c r="J7" s="4"/>
@@ -2719,17 +2916,17 @@
     <row r="8" ht="14.25" customHeight="1">
       <c r="A8" s="4"/>
       <c r="B8" s="6" t="s">
-        <v>85</v>
+        <v>106</v>
       </c>
       <c r="C8" s="7"/>
       <c r="D8" s="7"/>
       <c r="E8" s="8"/>
-      <c r="F8" s="30">
+      <c r="F8" s="36">
         <f>SUM(F3:F7)</f>
         <v>0</v>
       </c>
       <c r="H8" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="I8" s="4"/>
       <c r="J8" s="4"/>
@@ -2738,145 +2935,145 @@
     <row r="9" ht="14.25" customHeight="1"/>
     <row r="10" ht="14.25" customHeight="1"/>
     <row r="11" ht="14.25" customHeight="1">
-      <c r="A11" s="14" t="s">
-        <v>70</v>
-      </c>
-      <c r="B11" s="14" t="s">
-        <v>71</v>
-      </c>
-      <c r="C11" s="14" t="s">
-        <v>72</v>
-      </c>
-      <c r="D11" s="12" t="s">
-        <v>86</v>
-      </c>
-      <c r="E11" s="14" t="s">
-        <v>74</v>
-      </c>
-      <c r="F11" s="14" t="s">
-        <v>87</v>
-      </c>
-      <c r="H11" s="26" t="s">
-        <v>88</v>
-      </c>
-      <c r="I11" s="28"/>
+      <c r="A11" s="16" t="s">
+        <v>91</v>
+      </c>
+      <c r="B11" s="16" t="s">
+        <v>92</v>
+      </c>
+      <c r="C11" s="16" t="s">
+        <v>93</v>
+      </c>
+      <c r="D11" s="14" t="s">
+        <v>107</v>
+      </c>
+      <c r="E11" s="16" t="s">
+        <v>95</v>
+      </c>
+      <c r="F11" s="16" t="s">
+        <v>108</v>
+      </c>
+      <c r="H11" s="32" t="s">
+        <v>109</v>
+      </c>
+      <c r="I11" s="34"/>
     </row>
     <row r="12" ht="14.25" customHeight="1">
       <c r="A12" s="4" t="s">
-        <v>77</v>
+        <v>98</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C12" s="4"/>
       <c r="D12" s="4"/>
-      <c r="E12" s="29">
+      <c r="E12" s="35">
         <v>0.0</v>
       </c>
-      <c r="F12" s="30">
+      <c r="F12" s="36">
         <f t="shared" ref="F12:F16" si="2">D12*E12</f>
         <v>0</v>
       </c>
       <c r="H12" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="I12" s="30">
+        <v>7</v>
+      </c>
+      <c r="I12" s="36">
         <f t="shared" ref="I12:I16" si="3">F3+F12+F21+F30+F39</f>
         <v>0</v>
       </c>
     </row>
     <row r="13" ht="14.25" customHeight="1">
       <c r="A13" s="4" t="s">
-        <v>80</v>
+        <v>101</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C13" s="31"/>
+        <v>8</v>
+      </c>
+      <c r="C13" s="37"/>
       <c r="D13" s="4"/>
-      <c r="E13" s="29">
+      <c r="E13" s="35">
         <v>0.0</v>
       </c>
-      <c r="F13" s="30">
+      <c r="F13" s="36">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="H13" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="I13" s="30">
+        <v>8</v>
+      </c>
+      <c r="I13" s="36">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
     <row r="14" ht="14.25" customHeight="1">
       <c r="A14" s="4" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>81</v>
+        <v>102</v>
       </c>
       <c r="C14" s="4"/>
       <c r="D14" s="4"/>
-      <c r="E14" s="29">
+      <c r="E14" s="35">
         <v>0.0</v>
       </c>
-      <c r="F14" s="30">
+      <c r="F14" s="36">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="H14" s="4" t="s">
-        <v>83</v>
-      </c>
-      <c r="I14" s="30">
+        <v>104</v>
+      </c>
+      <c r="I14" s="36">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
     <row r="15" ht="14.25" customHeight="1">
       <c r="A15" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>82</v>
+        <v>103</v>
       </c>
       <c r="C15" s="4"/>
       <c r="D15" s="4"/>
-      <c r="E15" s="29">
+      <c r="E15" s="35">
         <v>0.0</v>
       </c>
-      <c r="F15" s="30">
+      <c r="F15" s="36">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="H15" s="4" t="s">
-        <v>82</v>
-      </c>
-      <c r="I15" s="30">
+        <v>103</v>
+      </c>
+      <c r="I15" s="36">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
     <row r="16" ht="14.25" customHeight="1">
       <c r="A16" s="4" t="s">
-        <v>84</v>
+        <v>105</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C16" s="4"/>
       <c r="D16" s="4"/>
-      <c r="E16" s="29">
+      <c r="E16" s="35">
         <v>0.0</v>
       </c>
-      <c r="F16" s="30">
+      <c r="F16" s="36">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="H16" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="I16" s="30">
+        <v>11</v>
+      </c>
+      <c r="I16" s="36">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
@@ -2884,19 +3081,19 @@
     <row r="17" ht="14.25" customHeight="1">
       <c r="A17" s="4"/>
       <c r="B17" s="6" t="s">
-        <v>89</v>
+        <v>110</v>
       </c>
       <c r="C17" s="7"/>
       <c r="D17" s="7"/>
       <c r="E17" s="8"/>
-      <c r="F17" s="30">
+      <c r="F17" s="36">
         <f>SUM(F12:F16)</f>
         <v>0</v>
       </c>
-      <c r="H17" s="32" t="s">
-        <v>90</v>
-      </c>
-      <c r="I17" s="33">
+      <c r="H17" s="38" t="s">
+        <v>111</v>
+      </c>
+      <c r="I17" s="39">
         <f>SUM(I12:I16)</f>
         <v>0</v>
       </c>
@@ -2904,145 +3101,145 @@
     <row r="18" ht="14.25" customHeight="1"/>
     <row r="19" ht="14.25" customHeight="1"/>
     <row r="20" ht="14.25" customHeight="1">
-      <c r="A20" s="14" t="s">
-        <v>70</v>
-      </c>
-      <c r="B20" s="14" t="s">
-        <v>71</v>
-      </c>
-      <c r="C20" s="14" t="s">
-        <v>72</v>
-      </c>
-      <c r="D20" s="12" t="s">
-        <v>86</v>
-      </c>
-      <c r="E20" s="14" t="s">
-        <v>74</v>
-      </c>
-      <c r="F20" s="14" t="s">
+      <c r="A20" s="16" t="s">
         <v>91</v>
       </c>
-      <c r="H20" s="26" t="s">
+      <c r="B20" s="16" t="s">
         <v>92</v>
       </c>
-      <c r="I20" s="28"/>
+      <c r="C20" s="16" t="s">
+        <v>93</v>
+      </c>
+      <c r="D20" s="14" t="s">
+        <v>107</v>
+      </c>
+      <c r="E20" s="16" t="s">
+        <v>95</v>
+      </c>
+      <c r="F20" s="16" t="s">
+        <v>112</v>
+      </c>
+      <c r="H20" s="32" t="s">
+        <v>113</v>
+      </c>
+      <c r="I20" s="34"/>
     </row>
     <row r="21" ht="14.25" customHeight="1">
       <c r="A21" s="4" t="s">
-        <v>77</v>
+        <v>98</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C21" s="4"/>
       <c r="D21" s="4"/>
-      <c r="E21" s="29">
+      <c r="E21" s="35">
         <v>0.0</v>
       </c>
-      <c r="F21" s="30">
+      <c r="F21" s="36">
         <f t="shared" ref="F21:F25" si="4">D21*E21</f>
         <v>0</v>
       </c>
       <c r="H21" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="I21" s="30">
+        <v>6</v>
+      </c>
+      <c r="I21" s="36">
         <f>F8</f>
         <v>0</v>
       </c>
     </row>
     <row r="22" ht="14.25" customHeight="1">
       <c r="A22" s="4" t="s">
-        <v>80</v>
+        <v>101</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C22" s="31"/>
+        <v>8</v>
+      </c>
+      <c r="C22" s="37"/>
       <c r="D22" s="4"/>
-      <c r="E22" s="29">
+      <c r="E22" s="35">
         <v>0.0</v>
       </c>
-      <c r="F22" s="30">
+      <c r="F22" s="36">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="H22" s="4" t="s">
-        <v>93</v>
-      </c>
-      <c r="I22" s="30">
+        <v>114</v>
+      </c>
+      <c r="I22" s="36">
         <f>F17</f>
         <v>0</v>
       </c>
     </row>
     <row r="23" ht="14.25" customHeight="1">
       <c r="A23" s="4" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>81</v>
+        <v>102</v>
       </c>
       <c r="C23" s="4"/>
       <c r="D23" s="4"/>
-      <c r="E23" s="29">
+      <c r="E23" s="35">
         <v>0.0</v>
       </c>
-      <c r="F23" s="30">
+      <c r="F23" s="36">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="H23" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="I23" s="30">
+        <v>54</v>
+      </c>
+      <c r="I23" s="36">
         <f>F26</f>
         <v>0</v>
       </c>
     </row>
     <row r="24" ht="14.25" customHeight="1">
       <c r="A24" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>82</v>
+        <v>103</v>
       </c>
       <c r="C24" s="4"/>
       <c r="D24" s="4"/>
-      <c r="E24" s="29">
+      <c r="E24" s="35">
         <v>0.0</v>
       </c>
-      <c r="F24" s="30">
+      <c r="F24" s="36">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="H24" s="4" t="s">
-        <v>94</v>
-      </c>
-      <c r="I24" s="30">
+        <v>115</v>
+      </c>
+      <c r="I24" s="36">
         <f>F35</f>
         <v>0</v>
       </c>
     </row>
     <row r="25" ht="14.25" customHeight="1">
       <c r="A25" s="4" t="s">
-        <v>84</v>
+        <v>105</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C25" s="4"/>
       <c r="D25" s="4"/>
-      <c r="E25" s="29">
+      <c r="E25" s="35">
         <v>0.0</v>
       </c>
-      <c r="F25" s="30">
+      <c r="F25" s="36">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="H25" s="4" t="s">
-        <v>95</v>
-      </c>
-      <c r="I25" s="30">
+        <v>116</v>
+      </c>
+      <c r="I25" s="36">
         <f>F44</f>
         <v>0</v>
       </c>
@@ -3050,19 +3247,19 @@
     <row r="26" ht="14.25" customHeight="1">
       <c r="A26" s="4"/>
       <c r="B26" s="6" t="s">
-        <v>96</v>
+        <v>117</v>
       </c>
       <c r="C26" s="7"/>
       <c r="D26" s="7"/>
       <c r="E26" s="8"/>
-      <c r="F26" s="30">
+      <c r="F26" s="36">
         <f>SUM(F21:F25)</f>
         <v>0</v>
       </c>
-      <c r="H26" s="32" t="s">
-        <v>97</v>
-      </c>
-      <c r="I26" s="33">
+      <c r="H26" s="38" t="s">
+        <v>118</v>
+      </c>
+      <c r="I26" s="39">
         <f>SUM(I21:I25)</f>
         <v>0</v>
       </c>
@@ -3070,136 +3267,136 @@
     <row r="27" ht="14.25" customHeight="1"/>
     <row r="28" ht="14.25" customHeight="1"/>
     <row r="29" ht="14.25" customHeight="1">
-      <c r="A29" s="14" t="s">
-        <v>70</v>
-      </c>
-      <c r="B29" s="14" t="s">
-        <v>71</v>
-      </c>
-      <c r="C29" s="14" t="s">
-        <v>72</v>
-      </c>
-      <c r="D29" s="12" t="s">
-        <v>86</v>
-      </c>
-      <c r="E29" s="14" t="s">
-        <v>74</v>
-      </c>
-      <c r="F29" s="14" t="s">
-        <v>98</v>
-      </c>
-      <c r="H29" s="14" t="s">
-        <v>99</v>
-      </c>
-      <c r="I29" s="34">
+      <c r="A29" s="16" t="s">
+        <v>91</v>
+      </c>
+      <c r="B29" s="16" t="s">
+        <v>92</v>
+      </c>
+      <c r="C29" s="16" t="s">
+        <v>93</v>
+      </c>
+      <c r="D29" s="14" t="s">
+        <v>107</v>
+      </c>
+      <c r="E29" s="16" t="s">
+        <v>95</v>
+      </c>
+      <c r="F29" s="16" t="s">
+        <v>119</v>
+      </c>
+      <c r="H29" s="16" t="s">
+        <v>120</v>
+      </c>
+      <c r="I29" s="40">
         <v>0.6</v>
       </c>
     </row>
     <row r="30" ht="14.25" customHeight="1">
       <c r="A30" s="4" t="s">
-        <v>77</v>
+        <v>98</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C30" s="4" t="s">
-        <v>100</v>
+        <v>121</v>
       </c>
       <c r="D30" s="4"/>
-      <c r="E30" s="29">
+      <c r="E30" s="35">
         <v>0.0</v>
       </c>
-      <c r="F30" s="30">
+      <c r="F30" s="36">
         <f t="shared" ref="F30:F34" si="5">D30*E30</f>
         <v>0</v>
       </c>
       <c r="H30" s="4" t="s">
-        <v>101</v>
-      </c>
-      <c r="I30" s="30">
+        <v>122</v>
+      </c>
+      <c r="I30" s="36">
         <f>I26*I29</f>
         <v>0</v>
       </c>
     </row>
     <row r="31" ht="14.25" customHeight="1">
       <c r="A31" s="4" t="s">
-        <v>80</v>
+        <v>101</v>
       </c>
       <c r="B31" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C31" s="31" t="s">
-        <v>102</v>
+        <v>8</v>
+      </c>
+      <c r="C31" s="37" t="s">
+        <v>123</v>
       </c>
       <c r="D31" s="4"/>
-      <c r="E31" s="29">
+      <c r="E31" s="35">
         <v>0.0</v>
       </c>
-      <c r="F31" s="30">
+      <c r="F31" s="36">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="H31" s="4" t="s">
-        <v>103</v>
-      </c>
-      <c r="I31" s="30">
+        <v>124</v>
+      </c>
+      <c r="I31" s="36">
         <f>I26+I30</f>
         <v>0</v>
       </c>
     </row>
     <row r="32" ht="14.25" customHeight="1">
       <c r="A32" s="4" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B32" s="4" t="s">
-        <v>81</v>
+        <v>102</v>
       </c>
       <c r="C32" s="4" t="s">
-        <v>104</v>
+        <v>125</v>
       </c>
       <c r="D32" s="4"/>
-      <c r="E32" s="29">
+      <c r="E32" s="35">
         <v>0.0</v>
       </c>
-      <c r="F32" s="30">
+      <c r="F32" s="36">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
     <row r="33" ht="14.25" customHeight="1">
       <c r="A33" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B33" s="4" t="s">
-        <v>82</v>
+        <v>103</v>
       </c>
       <c r="C33" s="4" t="s">
-        <v>105</v>
+        <v>126</v>
       </c>
       <c r="D33" s="4"/>
-      <c r="E33" s="29">
+      <c r="E33" s="35">
         <v>0.0</v>
       </c>
-      <c r="F33" s="30">
+      <c r="F33" s="36">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
     <row r="34" ht="14.25" customHeight="1">
       <c r="A34" s="4" t="s">
-        <v>84</v>
+        <v>105</v>
       </c>
       <c r="B34" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C34" s="4" t="s">
-        <v>105</v>
+        <v>126</v>
       </c>
       <c r="D34" s="4"/>
-      <c r="E34" s="29">
+      <c r="E34" s="35">
         <v>0.0</v>
       </c>
-      <c r="F34" s="30">
+      <c r="F34" s="36">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
@@ -3207,12 +3404,12 @@
     <row r="35" ht="14.25" customHeight="1">
       <c r="A35" s="4"/>
       <c r="B35" s="6" t="s">
-        <v>106</v>
+        <v>127</v>
       </c>
       <c r="C35" s="7"/>
       <c r="D35" s="7"/>
       <c r="E35" s="8"/>
-      <c r="F35" s="30">
+      <c r="F35" s="36">
         <f>SUM(F30:F34)</f>
         <v>0</v>
       </c>
@@ -3220,116 +3417,116 @@
     <row r="36" ht="14.25" customHeight="1"/>
     <row r="37" ht="14.25" customHeight="1"/>
     <row r="38" ht="14.25" customHeight="1">
-      <c r="A38" s="14" t="s">
-        <v>70</v>
-      </c>
-      <c r="B38" s="14" t="s">
-        <v>71</v>
-      </c>
-      <c r="C38" s="14" t="s">
-        <v>72</v>
-      </c>
-      <c r="D38" s="12" t="s">
-        <v>86</v>
-      </c>
-      <c r="E38" s="14" t="s">
-        <v>74</v>
-      </c>
-      <c r="F38" s="12" t="s">
+      <c r="A38" s="16" t="s">
+        <v>91</v>
+      </c>
+      <c r="B38" s="16" t="s">
+        <v>92</v>
+      </c>
+      <c r="C38" s="16" t="s">
+        <v>93</v>
+      </c>
+      <c r="D38" s="14" t="s">
         <v>107</v>
+      </c>
+      <c r="E38" s="16" t="s">
+        <v>95</v>
+      </c>
+      <c r="F38" s="14" t="s">
+        <v>128</v>
       </c>
     </row>
     <row r="39" ht="14.25" customHeight="1">
       <c r="A39" s="4" t="s">
-        <v>77</v>
+        <v>98</v>
       </c>
       <c r="B39" s="4" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C39" s="4" t="s">
-        <v>100</v>
+        <v>121</v>
       </c>
       <c r="D39" s="4"/>
-      <c r="E39" s="29">
+      <c r="E39" s="35">
         <v>0.0</v>
       </c>
-      <c r="F39" s="30">
+      <c r="F39" s="36">
         <f t="shared" ref="F39:F43" si="6">D39*E39</f>
         <v>0</v>
       </c>
     </row>
     <row r="40" ht="14.25" customHeight="1">
       <c r="A40" s="4" t="s">
-        <v>80</v>
+        <v>101</v>
       </c>
       <c r="B40" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C40" s="31" t="s">
-        <v>102</v>
+        <v>8</v>
+      </c>
+      <c r="C40" s="37" t="s">
+        <v>123</v>
       </c>
       <c r="D40" s="4"/>
-      <c r="E40" s="29">
+      <c r="E40" s="35">
         <v>0.0</v>
       </c>
-      <c r="F40" s="30">
+      <c r="F40" s="36">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
     </row>
     <row r="41" ht="14.25" customHeight="1">
       <c r="A41" s="4" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B41" s="4" t="s">
-        <v>81</v>
+        <v>102</v>
       </c>
       <c r="C41" s="4" t="s">
-        <v>104</v>
+        <v>125</v>
       </c>
       <c r="D41" s="4"/>
-      <c r="E41" s="29">
+      <c r="E41" s="35">
         <v>0.0</v>
       </c>
-      <c r="F41" s="30">
+      <c r="F41" s="36">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
     </row>
     <row r="42" ht="14.25" customHeight="1">
       <c r="A42" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B42" s="4" t="s">
-        <v>82</v>
+        <v>103</v>
       </c>
       <c r="C42" s="4" t="s">
-        <v>105</v>
+        <v>126</v>
       </c>
       <c r="D42" s="4"/>
-      <c r="E42" s="29">
+      <c r="E42" s="35">
         <v>0.0</v>
       </c>
-      <c r="F42" s="30">
+      <c r="F42" s="36">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
     </row>
     <row r="43" ht="14.25" customHeight="1">
       <c r="A43" s="4" t="s">
-        <v>84</v>
+        <v>105</v>
       </c>
       <c r="B43" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C43" s="4" t="s">
-        <v>105</v>
+        <v>126</v>
       </c>
       <c r="D43" s="4"/>
-      <c r="E43" s="29">
+      <c r="E43" s="35">
         <v>0.0</v>
       </c>
-      <c r="F43" s="30">
+      <c r="F43" s="36">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
@@ -3337,12 +3534,12 @@
     <row r="44" ht="14.25" customHeight="1">
       <c r="A44" s="4"/>
       <c r="B44" s="6" t="s">
-        <v>108</v>
+        <v>129</v>
       </c>
       <c r="C44" s="7"/>
       <c r="D44" s="7"/>
       <c r="E44" s="8"/>
-      <c r="F44" s="30">
+      <c r="F44" s="36">
         <f>SUM(F39:F43)</f>
         <v>0</v>
       </c>

</xml_diff>

<commit_message>
Actualizando docuemento para entrega
</commit_message>
<xml_diff>
--- a/FASE1/DOCS/EVIDENCIAS_GRUPALES/ENTREGABLES/Matriz EDT.xlsx
+++ b/FASE1/DOCS/EVIDENCIAS_GRUPALES/ENTREGABLES/Matriz EDT.xlsx
@@ -10,14 +10,14 @@
   <calcPr/>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion2">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId6" roundtripDataChecksum="LeARRrPx/uazhj5IN+gtJBd9W6McP4tE1kMCkYT5Srg="/>
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId6" roundtripDataChecksum="Dy/DENlDh5z8zA3RSThAi5izNAnBbVufUTiFCY0+bcM="/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="246" uniqueCount="130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="367" uniqueCount="151">
   <si>
     <t>Matriz Estructura de descomposición de tareas EDT</t>
   </si>
@@ -34,9 +34,6 @@
     <t>DICCIONARIO EDT</t>
   </si>
   <si>
-    <t>columna con valores de tarea</t>
-  </si>
-  <si>
     <t>Fase de Planificación</t>
   </si>
   <si>
@@ -70,7 +67,10 @@
     <t>Acta de Constitución de proyecto</t>
   </si>
   <si>
-    <t>S1</t>
+    <t>S1-S2</t>
+  </si>
+  <si>
+    <t>8hrs</t>
   </si>
   <si>
     <t xml:space="preserve">Jefe de Proyecto </t>
@@ -79,163 +79,196 @@
     <t>Matias Acuna -</t>
   </si>
   <si>
-    <t>Sueldo diario = $68.182</t>
-  </si>
-  <si>
-    <t>$1.500.000</t>
-  </si>
-  <si>
-    <t>$600.000</t>
+    <t>Sueldo por hora= $1416</t>
   </si>
   <si>
     <t>Organización del equipo</t>
   </si>
   <si>
-    <t xml:space="preserve">S1 </t>
+    <t>S3</t>
+  </si>
+  <si>
+    <t>2hrs</t>
+  </si>
+  <si>
+    <t>2h</t>
   </si>
   <si>
     <t>Fabian Carrasco</t>
   </si>
   <si>
-    <t>Valor hora (8hr) = $8.523</t>
-  </si>
-  <si>
-    <t>$1.500.001</t>
-  </si>
-  <si>
-    <t>$750.000</t>
+    <t>Valor por hora = $8.523</t>
   </si>
   <si>
     <t>Definición de requerimientos Generales</t>
   </si>
   <si>
-    <t>S2</t>
-  </si>
-  <si>
     <t>Matias Acuna</t>
   </si>
   <si>
-    <t>Valor hora (9hr) = $7.526</t>
-  </si>
-  <si>
-    <t>$1.500.002</t>
+    <t>Valor por hora =$7.689</t>
   </si>
   <si>
     <t>Aprobación acta de constitución</t>
   </si>
   <si>
-    <t>$1.500.003</t>
-  </si>
-  <si>
-    <t>$150.000</t>
-  </si>
-  <si>
-    <t>$1.500.004</t>
+    <t>4hrs</t>
+  </si>
+  <si>
+    <t>Constanza Munoz</t>
+  </si>
+  <si>
+    <t>Valor por hora = $6.666</t>
+  </si>
+  <si>
+    <t>Total primera Fase</t>
+  </si>
+  <si>
+    <t>18hrs</t>
+  </si>
+  <si>
+    <t>14hrs</t>
+  </si>
+  <si>
+    <t>Valor por hora =$7.582</t>
   </si>
   <si>
     <t>Fase de Análisis y diseño</t>
   </si>
   <si>
-    <t>Constanza Munoz</t>
-  </si>
-  <si>
-    <t>$1.500.005</t>
+    <t>Valor por hora  =$14.583</t>
   </si>
   <si>
     <t xml:space="preserve">Captura de requerimientos específicos </t>
   </si>
   <si>
-    <t>S3</t>
+    <t>S3-S4</t>
   </si>
   <si>
     <t>Documento de arquitectura SW</t>
   </si>
   <si>
-    <t>S3 - S4</t>
-  </si>
-  <si>
-    <t>%</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Regla de reparto % horas trabajadas </t>
+    <t>S3 -S4-S5</t>
   </si>
   <si>
     <t>Documento de casos de uso</t>
   </si>
   <si>
+    <t>Prototipos</t>
+  </si>
+  <si>
     <t>S4 - S5</t>
   </si>
   <si>
-    <t>Prototipos</t>
-  </si>
-  <si>
-    <t>S5 - S6</t>
-  </si>
-  <si>
-    <t>abarcar sueldos</t>
+    <t>10hrs</t>
   </si>
   <si>
     <t>Propuesta ERS</t>
   </si>
   <si>
+    <t>S5</t>
+  </si>
+  <si>
+    <t>Total Segunda Fase</t>
+  </si>
+  <si>
+    <t>44hrs</t>
+  </si>
+  <si>
+    <t>Fase de Desarrollo</t>
+  </si>
+  <si>
+    <t>Implementación ambiente de desarrollo</t>
+  </si>
+  <si>
     <t>S6</t>
   </si>
   <si>
-    <t>Fase de Desarrollo</t>
-  </si>
-  <si>
-    <t>Implementación ambiente de desarrollo</t>
+    <t>Scripts de base de datos (tablas, relaciones)</t>
+  </si>
+  <si>
+    <t>S6-S7</t>
+  </si>
+  <si>
+    <t>Desarrollo sistema de registro de usuarios</t>
   </si>
   <si>
     <t>S7</t>
   </si>
   <si>
-    <t>Scripts de base de datos (tablas, relaciones)</t>
-  </si>
-  <si>
-    <t>S7 - S8</t>
-  </si>
-  <si>
-    <t>Desarrollo sistema de registro de usuarios</t>
-  </si>
-  <si>
     <t>Desarrollo sistem de autenticacion y roles</t>
   </si>
   <si>
+    <t>S7-S8</t>
+  </si>
+  <si>
     <t>Desarrollo Catalogo de productos filtrables</t>
   </si>
   <si>
+    <t>S8-S9</t>
+  </si>
+  <si>
     <t>Desarrollo flujo carro de compras</t>
   </si>
   <si>
     <t>Desarrollo de sistema de pedidos y seguimiento</t>
   </si>
   <si>
+    <t>S9</t>
+  </si>
+  <si>
     <t>Desarrollo BackOffice sistema de registro de usuarios</t>
   </si>
   <si>
+    <t>S9-S10</t>
+  </si>
+  <si>
     <t>Desarrollo BackOffice sistema de autenticacion y roles</t>
   </si>
   <si>
+    <t>S10-S11</t>
+  </si>
+  <si>
     <t>Desarrollo BackOffice catalogo de productos filtrables</t>
   </si>
   <si>
     <t>Desarrollo BackOffice flujo carro de compras</t>
   </si>
   <si>
+    <t>S11-S12-S13</t>
+  </si>
+  <si>
+    <t>12hrs</t>
+  </si>
+  <si>
     <t>Desarrollo BackOffice sistema de pedidos y seguimiento</t>
   </si>
   <si>
+    <t>S13-S14</t>
+  </si>
+  <si>
     <t>Notificaciones por correo (registro, compra, estado pedido)</t>
   </si>
   <si>
-    <t>S10 - S11</t>
+    <t>S14- S15</t>
+  </si>
+  <si>
+    <t>6hrs</t>
   </si>
   <si>
     <t>Reportes PDF/XLS</t>
   </si>
   <si>
-    <t>S11</t>
+    <t>S14-S15</t>
+  </si>
+  <si>
+    <t>Total Tercera Fase</t>
+  </si>
+  <si>
+    <t>64hrs</t>
+  </si>
+  <si>
+    <t>40hrs</t>
   </si>
   <si>
     <t>Fase de Pruebas y QA</t>
@@ -244,19 +277,31 @@
     <t>Implementación ambiente de pruebas</t>
   </si>
   <si>
-    <t>S12</t>
+    <t>S15</t>
   </si>
   <si>
     <t>Pruebas Funcionales</t>
   </si>
   <si>
-    <t>S12 - S13</t>
+    <t>S15-s16</t>
+  </si>
+  <si>
+    <t>Pruebas de integración</t>
+  </si>
+  <si>
+    <t>s16-s17</t>
   </si>
   <si>
     <t>Pruebas con Usuarios</t>
   </si>
   <si>
-    <t>S14</t>
+    <t>S17</t>
+  </si>
+  <si>
+    <t>Total Cuarta Fase</t>
+  </si>
+  <si>
+    <t>28hrs</t>
   </si>
   <si>
     <t>Fase de implementación y cierre</t>
@@ -265,31 +310,25 @@
     <t>Migración del sistema a producción</t>
   </si>
   <si>
-    <t>S15</t>
-  </si>
-  <si>
     <t>Capacitaciones</t>
   </si>
   <si>
-    <t>S16</t>
-  </si>
-  <si>
     <t>Manuales Usuario</t>
   </si>
   <si>
-    <t>S16 - S17</t>
-  </si>
-  <si>
     <t>Acta cierre de proyecto</t>
   </si>
   <si>
-    <t>S17</t>
-  </si>
-  <si>
     <t>Entrega final + documentación + presentación</t>
   </si>
   <si>
-    <t>S18</t>
+    <t>Total Quinta Fase</t>
+  </si>
+  <si>
+    <t>22hrs</t>
+  </si>
+  <si>
+    <t>16hrs</t>
   </si>
   <si>
     <t>SIGLA</t>
@@ -313,13 +352,31 @@
     <t>COSTO POR HORA</t>
   </si>
   <si>
+    <t>SUELDO MES</t>
+  </si>
+  <si>
     <t>JP</t>
   </si>
   <si>
+    <t>Matias Acuña</t>
+  </si>
+  <si>
     <t>COSTO x HORA</t>
   </si>
   <si>
-    <t>Sueldo mes</t>
+    <t>Sueldo Agos</t>
+  </si>
+  <si>
+    <t>Sueldo Sep</t>
+  </si>
+  <si>
+    <t>Sueldo Oct</t>
+  </si>
+  <si>
+    <t>Sueldo Nov</t>
+  </si>
+  <si>
+    <t>Sueldo Dic</t>
   </si>
   <si>
     <t>AP</t>
@@ -331,22 +388,37 @@
     <t>Calidad Y Testing</t>
   </si>
   <si>
+    <t>Constanza Muñoz</t>
+  </si>
+  <si>
     <t>Administrador BD</t>
   </si>
   <si>
+    <t>DG</t>
+  </si>
+  <si>
+    <t>Diseño</t>
+  </si>
+  <si>
+    <t>Project Managment</t>
+  </si>
+  <si>
+    <t>TOTAL FASE PLANIFICACION</t>
+  </si>
+  <si>
+    <t xml:space="preserve">VALOR HORA HH </t>
+  </si>
+  <si>
+    <t>FASE DISEÑO</t>
+  </si>
+  <si>
+    <t>COSTO HH POR ROL</t>
+  </si>
+  <si>
     <t>DI</t>
   </si>
   <si>
-    <t>TOTAL FASE PLANIFICACION</t>
-  </si>
-  <si>
-    <t xml:space="preserve">VALOR HORA HH </t>
-  </si>
-  <si>
-    <t>FASE DISEÑO</t>
-  </si>
-  <si>
-    <t>COSTO HH POR ROL</t>
+    <t>PM</t>
   </si>
   <si>
     <t>TOTAL FASE DISEÑO</t>
@@ -370,6 +442,9 @@
     <t>Fase de Implementación y Cierre</t>
   </si>
   <si>
+    <t>Constabza Muñoz</t>
+  </si>
+  <si>
     <t>TOTAL FASE DESARROLLO</t>
   </si>
   <si>
@@ -382,22 +457,10 @@
     <t xml:space="preserve">Margen </t>
   </si>
   <si>
-    <t>Jeanette Leonelli</t>
-  </si>
-  <si>
     <t>UTILIDAD</t>
   </si>
   <si>
-    <t>Alan Gajardo</t>
-  </si>
-  <si>
     <t>PRECIO FINAL</t>
-  </si>
-  <si>
-    <t>Pavel Bustamante</t>
-  </si>
-  <si>
-    <t>Victor Vasquez</t>
   </si>
   <si>
     <t>TOTAL FASE PRUEBAS QA</t>
@@ -436,14 +499,14 @@
       <name val="Calibri"/>
     </font>
     <font>
+      <sz val="11.0"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
       <color theme="1"/>
       <name val="Calibri"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11.0"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
     </font>
     <font>
       <b/>
@@ -604,7 +667,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="45">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -628,9 +691,6 @@
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
     <xf borderId="8" fillId="3" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFill="1" applyFont="1"/>
     <xf borderId="4" fillId="3" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="4" fillId="3" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
@@ -645,10 +705,10 @@
     <xf borderId="4" fillId="3" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="3" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="4" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf borderId="9" fillId="4" fontId="5" numFmtId="0" xfId="0" applyBorder="1" applyFill="1" applyFont="1"/>
+    <xf borderId="9" fillId="4" fontId="4" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="4" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
@@ -658,7 +718,7 @@
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="9" fillId="4" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="9" fillId="4" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="4" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
@@ -667,32 +727,45 @@
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
     </xf>
-    <xf borderId="10" fillId="4" fontId="5" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="4" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="10" fillId="4" fontId="4" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="5" fillId="4" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="5" fillId="4" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="4" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
     </xf>
-    <xf borderId="9" fillId="4" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="9" fillId="4" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="left"/>
     </xf>
     <xf borderId="4" fillId="0" fontId="3" numFmtId="9" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="9" fillId="4" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0"/>
     </xf>
     <xf borderId="11" fillId="3" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center"/>
     </xf>
     <xf borderId="12" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="13" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="11" fillId="3" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0"/>
+    </xf>
+    <xf borderId="4" fillId="0" fontId="3" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="4" fillId="0" fontId="3" numFmtId="165" xfId="0" applyBorder="1" applyFont="1" applyNumberFormat="1"/>
+    <xf borderId="4" fillId="0" fontId="3" numFmtId="165" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="4" fillId="0" fontId="5" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="4" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
     <xf borderId="4" fillId="0" fontId="3" numFmtId="164" xfId="0" applyBorder="1" applyFont="1" applyNumberFormat="1"/>
-    <xf borderId="4" fillId="0" fontId="3" numFmtId="165" xfId="0" applyBorder="1" applyFont="1" applyNumberFormat="1"/>
-    <xf borderId="4" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment shrinkToFit="0" wrapText="1"/>
-    </xf>
     <xf borderId="4" fillId="5" fontId="6" numFmtId="0" xfId="0" applyBorder="1" applyFill="1" applyFont="1"/>
     <xf borderId="4" fillId="5" fontId="6" numFmtId="165" xfId="0" applyBorder="1" applyFont="1" applyNumberFormat="1"/>
     <xf borderId="4" fillId="0" fontId="3" numFmtId="9" xfId="0" applyBorder="1" applyFont="1" applyNumberFormat="1"/>
@@ -923,10 +996,11 @@
     <col customWidth="1" min="5" max="5" width="9.14"/>
     <col customWidth="1" min="6" max="6" width="8.14"/>
     <col customWidth="1" min="7" max="8" width="12.0"/>
-    <col customWidth="1" min="9" max="9" width="5.0"/>
-    <col customWidth="1" min="10" max="10" width="23.29"/>
-    <col customWidth="1" min="11" max="13" width="31.57"/>
-    <col customWidth="1" min="14" max="29" width="10.71"/>
+    <col customWidth="1" min="9" max="9" width="11.43"/>
+    <col customWidth="1" min="10" max="11" width="16.0"/>
+    <col customWidth="1" min="12" max="12" width="23.29"/>
+    <col customWidth="1" min="13" max="15" width="31.57"/>
+    <col customWidth="1" min="16" max="31" width="10.71"/>
   </cols>
   <sheetData>
     <row r="1" ht="14.25" customHeight="1"/>
@@ -954,843 +1028,889 @@
       <c r="F4" s="7"/>
       <c r="G4" s="8"/>
       <c r="H4" s="9"/>
-      <c r="J4" s="6" t="s">
+      <c r="L4" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="K4" s="8"/>
-      <c r="L4" s="9"/>
-      <c r="M4" s="10"/>
-      <c r="P4" s="11" t="s">
+      <c r="M4" s="8"/>
+      <c r="N4" s="9"/>
+      <c r="O4" s="10"/>
+    </row>
+    <row r="5" ht="14.25" customHeight="1">
+      <c r="A5" s="11" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="5" ht="14.25" customHeight="1">
-      <c r="A5" s="12" t="s">
+      <c r="B5" s="12"/>
+      <c r="C5" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="13"/>
-      <c r="C5" s="14" t="s">
+      <c r="D5" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="D5" s="14" t="s">
+      <c r="E5" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="E5" s="14" t="s">
+      <c r="F5" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="F5" s="14" t="s">
+      <c r="G5" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="G5" s="14" t="s">
+      <c r="H5" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="H5" s="15" t="s">
+      <c r="L5" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="J5" s="16" t="s">
+      <c r="M5" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="K5" s="16" t="s">
+      <c r="N5" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="L5" s="17" t="s">
+      <c r="O5" s="17"/>
+    </row>
+    <row r="6" ht="14.25" customHeight="1" outlineLevel="1">
+      <c r="A6" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="M5" s="18"/>
-    </row>
-    <row r="6" ht="14.25" customHeight="1" outlineLevel="1">
-      <c r="A6" s="19" t="s">
+      <c r="B6" s="19" t="s">
         <v>16</v>
       </c>
-      <c r="B6" s="20" t="s">
+      <c r="C6" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="C6" s="21">
-        <v>0.4</v>
-      </c>
-      <c r="D6" s="21">
-        <v>0.5</v>
-      </c>
+      <c r="D6" s="5"/>
       <c r="E6" s="9"/>
-      <c r="F6" s="21">
-        <v>0.1</v>
-      </c>
+      <c r="F6" s="20"/>
       <c r="G6" s="9"/>
-      <c r="H6" s="5"/>
-      <c r="J6" s="20" t="s">
+      <c r="H6" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="L6" s="19" t="s">
         <v>18</v>
       </c>
-      <c r="K6" s="20" t="s">
+      <c r="M6" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="L6" s="20" t="s">
+      <c r="N6" s="19" t="s">
         <v>20</v>
       </c>
-      <c r="M6" s="22"/>
-      <c r="N6" s="11" t="s">
+      <c r="O6" s="21"/>
+    </row>
+    <row r="7" ht="14.25" customHeight="1" outlineLevel="1">
+      <c r="A7" s="22" t="s">
         <v>21</v>
       </c>
-      <c r="O6" s="11" t="s">
+      <c r="B7" s="19" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="7" ht="14.25" customHeight="1" outlineLevel="1">
-      <c r="A7" s="23" t="s">
+      <c r="C7" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="B7" s="20" t="s">
+      <c r="D7" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="E7" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="C7" s="21">
-        <v>0.4</v>
-      </c>
-      <c r="D7" s="21">
-        <v>0.5</v>
-      </c>
-      <c r="E7" s="9"/>
-      <c r="F7" s="21">
-        <v>0.1</v>
-      </c>
-      <c r="G7" s="9"/>
-      <c r="H7" s="5"/>
-      <c r="J7" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="K7" s="24" t="s">
+      <c r="F7" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="G7" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="H7" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="L7" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="M7" s="23" t="s">
         <v>25</v>
       </c>
-      <c r="L7" s="24" t="s">
+      <c r="N7" s="23" t="s">
         <v>26</v>
       </c>
-      <c r="M7" s="25"/>
-      <c r="N7" s="11" t="s">
+      <c r="O7" s="24"/>
+    </row>
+    <row r="8" ht="14.25" customHeight="1" outlineLevel="1">
+      <c r="A8" s="18" t="s">
         <v>27</v>
       </c>
-      <c r="O7" s="11" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="8" ht="14.25" customHeight="1" outlineLevel="1">
-      <c r="A8" s="19" t="s">
-        <v>29</v>
-      </c>
-      <c r="B8" s="20" t="s">
-        <v>30</v>
-      </c>
-      <c r="C8" s="21">
-        <v>0.4</v>
-      </c>
-      <c r="D8" s="21">
-        <v>0.5</v>
-      </c>
+      <c r="B8" s="19" t="s">
+        <v>22</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="D8" s="20"/>
       <c r="E8" s="9"/>
-      <c r="F8" s="21">
-        <v>0.1</v>
-      </c>
+      <c r="F8" s="20"/>
       <c r="G8" s="9"/>
       <c r="H8" s="5"/>
-      <c r="J8" s="4" t="s">
+      <c r="L8" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="M8" s="19" t="s">
+        <v>28</v>
+      </c>
+      <c r="N8" s="19" t="s">
+        <v>29</v>
+      </c>
+      <c r="O8" s="21"/>
+    </row>
+    <row r="9" ht="14.25" customHeight="1" outlineLevel="1">
+      <c r="A9" s="22" t="s">
+        <v>30</v>
+      </c>
+      <c r="B9" s="19" t="s">
+        <v>22</v>
+      </c>
+      <c r="C9" s="20"/>
+      <c r="D9" s="20"/>
+      <c r="E9" s="9"/>
+      <c r="F9" s="20"/>
+      <c r="G9" s="9"/>
+      <c r="H9" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="L9" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="K8" s="20" t="s">
-        <v>31</v>
-      </c>
-      <c r="L8" s="20" t="s">
+      <c r="M9" s="19" t="s">
         <v>32</v>
       </c>
-      <c r="M8" s="22"/>
-      <c r="N8" s="11" t="s">
+      <c r="N9" s="19" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="9" ht="14.25" customHeight="1" outlineLevel="1">
-      <c r="A9" s="23" t="s">
+      <c r="O9" s="21"/>
+    </row>
+    <row r="10" ht="14.25" customHeight="1" outlineLevel="1">
+      <c r="A10" s="19" t="s">
         <v>34</v>
       </c>
-      <c r="B9" s="20" t="s">
-        <v>30</v>
-      </c>
-      <c r="C9" s="21">
-        <v>0.4</v>
-      </c>
-      <c r="D9" s="21">
-        <v>0.5</v>
-      </c>
-      <c r="E9" s="9"/>
-      <c r="F9" s="21">
-        <v>0.1</v>
-      </c>
-      <c r="G9" s="9"/>
-      <c r="H9" s="5"/>
-      <c r="J9" s="4" t="s">
+      <c r="B10" s="4"/>
+      <c r="C10" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="E10" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="F10" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="G10" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="H10" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="L10" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="K9" s="20" t="s">
-        <v>25</v>
-      </c>
-      <c r="L9" s="20"/>
-      <c r="M9" s="22"/>
-      <c r="N9" s="11" t="s">
-        <v>35</v>
-      </c>
-      <c r="O9" s="11" t="s">
+      <c r="M10" s="19" t="s">
+        <v>28</v>
+      </c>
+      <c r="N10" s="19" t="s">
+        <v>37</v>
+      </c>
+      <c r="O10" s="21"/>
+    </row>
+    <row r="11" ht="14.25" customHeight="1">
+      <c r="A11" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="B11" s="12"/>
+      <c r="C11" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="D11" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="E11" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="F11" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="G11" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="H11" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="L11" s="19" t="s">
+        <v>11</v>
+      </c>
+      <c r="M11" s="19" t="s">
+        <v>32</v>
+      </c>
+      <c r="N11" s="19" t="s">
+        <v>39</v>
+      </c>
+      <c r="O11" s="21"/>
+    </row>
+    <row r="12" ht="14.25" customHeight="1" outlineLevel="1">
+      <c r="A12" s="18" t="s">
+        <v>40</v>
+      </c>
+      <c r="B12" s="19" t="s">
+        <v>41</v>
+      </c>
+      <c r="C12" s="20"/>
+      <c r="D12" s="20"/>
+      <c r="E12" s="9"/>
+      <c r="F12" s="20"/>
+      <c r="G12" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="H12" s="20"/>
+    </row>
+    <row r="13" ht="14.25" customHeight="1" outlineLevel="1">
+      <c r="A13" s="25" t="s">
+        <v>42</v>
+      </c>
+      <c r="B13" s="19" t="s">
+        <v>43</v>
+      </c>
+      <c r="C13" s="20"/>
+      <c r="D13" s="5" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="10" ht="14.25" customHeight="1" outlineLevel="1">
-      <c r="A10" s="4"/>
-      <c r="B10" s="4"/>
-      <c r="C10" s="9"/>
-      <c r="D10" s="9"/>
-      <c r="E10" s="9"/>
-      <c r="F10" s="9"/>
-      <c r="G10" s="9"/>
-      <c r="H10" s="9"/>
-      <c r="J10" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="K10" s="20" t="s">
-        <v>31</v>
-      </c>
-      <c r="L10" s="20"/>
-      <c r="M10" s="22"/>
-      <c r="N10" s="11" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="11" ht="14.25" customHeight="1">
-      <c r="A11" s="13" t="s">
-        <v>38</v>
-      </c>
-      <c r="B11" s="13"/>
-      <c r="C11" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="D11" s="14" t="s">
-        <v>8</v>
-      </c>
-      <c r="E11" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="F11" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="G11" s="14" t="s">
-        <v>11</v>
-      </c>
-      <c r="H11" s="15" t="s">
-        <v>12</v>
-      </c>
-      <c r="J11" s="20" t="s">
-        <v>12</v>
-      </c>
-      <c r="K11" s="20" t="s">
-        <v>39</v>
-      </c>
-      <c r="L11" s="20"/>
-      <c r="M11" s="22"/>
-      <c r="N11" s="11" t="s">
-        <v>40</v>
-      </c>
-      <c r="O11" s="11" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="12" ht="14.25" customHeight="1" outlineLevel="1">
-      <c r="A12" s="19" t="s">
+      <c r="E13" s="9"/>
+      <c r="F13" s="20"/>
+      <c r="G13" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="H13" s="20"/>
+      <c r="L13" s="26"/>
+      <c r="M13" s="26"/>
+      <c r="N13" s="26"/>
+      <c r="O13" s="26"/>
+    </row>
+    <row r="14" ht="14.25" customHeight="1" outlineLevel="1">
+      <c r="A14" s="18" t="s">
+        <v>44</v>
+      </c>
+      <c r="B14" s="19" t="s">
         <v>41</v>
       </c>
-      <c r="B12" s="20" t="s">
-        <v>42</v>
-      </c>
-      <c r="C12" s="21">
-        <v>0.35</v>
-      </c>
-      <c r="D12" s="21"/>
-      <c r="E12" s="9"/>
-      <c r="F12" s="21">
-        <v>0.2</v>
-      </c>
-      <c r="G12" s="9"/>
-      <c r="H12" s="21">
-        <v>0.45</v>
-      </c>
-    </row>
-    <row r="13" ht="14.25" customHeight="1" outlineLevel="1">
-      <c r="A13" s="26" t="s">
-        <v>43</v>
-      </c>
-      <c r="B13" s="20" t="s">
-        <v>44</v>
-      </c>
-      <c r="C13" s="21">
-        <v>0.6</v>
-      </c>
-      <c r="D13" s="21">
-        <v>0.15</v>
-      </c>
-      <c r="E13" s="9"/>
-      <c r="F13" s="21">
-        <v>0.25</v>
-      </c>
-      <c r="G13" s="9"/>
-      <c r="H13" s="21"/>
-      <c r="J13" s="27" t="s">
-        <v>45</v>
-      </c>
-      <c r="K13" s="27" t="s">
-        <v>46</v>
-      </c>
-      <c r="L13" s="11"/>
-      <c r="M13" s="11"/>
-    </row>
-    <row r="14" ht="14.25" customHeight="1" outlineLevel="1">
-      <c r="A14" s="19" t="s">
-        <v>47</v>
-      </c>
-      <c r="B14" s="20" t="s">
-        <v>48</v>
-      </c>
-      <c r="C14" s="21">
-        <v>0.35</v>
-      </c>
+      <c r="C14" s="20"/>
       <c r="D14" s="9"/>
       <c r="E14" s="9"/>
-      <c r="F14" s="21">
-        <v>0.2</v>
-      </c>
-      <c r="G14" s="9"/>
-      <c r="H14" s="21">
-        <v>0.45</v>
-      </c>
+      <c r="F14" s="20"/>
+      <c r="G14" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="H14" s="20"/>
     </row>
     <row r="15" ht="14.25" customHeight="1" outlineLevel="1">
-      <c r="A15" s="19" t="s">
-        <v>49</v>
-      </c>
-      <c r="B15" s="20" t="s">
-        <v>50</v>
-      </c>
-      <c r="C15" s="21">
-        <v>0.3</v>
-      </c>
+      <c r="A15" s="18" t="s">
+        <v>45</v>
+      </c>
+      <c r="B15" s="19" t="s">
+        <v>46</v>
+      </c>
+      <c r="C15" s="20"/>
       <c r="D15" s="5"/>
       <c r="E15" s="9"/>
-      <c r="F15" s="21">
-        <v>0.2</v>
-      </c>
-      <c r="G15" s="21">
-        <v>0.5</v>
-      </c>
-      <c r="H15" s="21"/>
-      <c r="J15" s="11" t="s">
-        <v>51</v>
-      </c>
+      <c r="F15" s="20"/>
+      <c r="G15" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="H15" s="20"/>
     </row>
     <row r="16" ht="14.25" customHeight="1" outlineLevel="1">
-      <c r="A16" s="19" t="s">
-        <v>52</v>
-      </c>
-      <c r="B16" s="20" t="s">
-        <v>53</v>
-      </c>
-      <c r="C16" s="21">
-        <v>0.35</v>
+      <c r="A16" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="B16" s="19" t="s">
+        <v>49</v>
+      </c>
+      <c r="C16" s="5" t="s">
+        <v>31</v>
       </c>
       <c r="D16" s="9"/>
       <c r="E16" s="9"/>
-      <c r="F16" s="21">
-        <v>0.2</v>
-      </c>
-      <c r="G16" s="9"/>
-      <c r="H16" s="21">
-        <v>0.45</v>
+      <c r="F16" s="20"/>
+      <c r="G16" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="H16" s="5" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="17" ht="14.25" customHeight="1" outlineLevel="1">
-      <c r="A17" s="4"/>
+      <c r="A17" s="19" t="s">
+        <v>50</v>
+      </c>
       <c r="B17" s="4"/>
-      <c r="C17" s="9"/>
-      <c r="D17" s="9"/>
+      <c r="C17" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="D17" s="5" t="s">
+        <v>36</v>
+      </c>
       <c r="E17" s="9"/>
       <c r="F17" s="9"/>
-      <c r="G17" s="9"/>
-      <c r="H17" s="9"/>
+      <c r="G17" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="H17" s="5" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="18" ht="14.25" customHeight="1">
-      <c r="A18" s="13" t="s">
+      <c r="A18" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="B18" s="12"/>
+      <c r="C18" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="D18" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="E18" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="F18" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="G18" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="H18" s="14" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="19" ht="18.0" customHeight="1" outlineLevel="1">
+      <c r="A19" s="18" t="s">
+        <v>53</v>
+      </c>
+      <c r="B19" s="19" t="s">
         <v>54</v>
       </c>
-      <c r="B18" s="13"/>
-      <c r="C18" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="D18" s="14" t="s">
-        <v>8</v>
-      </c>
-      <c r="E18" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="F18" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="G18" s="14" t="s">
-        <v>11</v>
-      </c>
-      <c r="H18" s="15" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="19" ht="18.0" customHeight="1" outlineLevel="1">
-      <c r="A19" s="19" t="s">
-        <v>55</v>
-      </c>
-      <c r="B19" s="20" t="s">
-        <v>56</v>
-      </c>
-      <c r="C19" s="21">
-        <v>0.2</v>
-      </c>
-      <c r="D19" s="21">
-        <v>0.6</v>
-      </c>
-      <c r="E19" s="21">
-        <v>0.05</v>
-      </c>
-      <c r="F19" s="21">
-        <v>0.15</v>
-      </c>
+      <c r="C19" s="5"/>
+      <c r="D19" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="E19" s="20"/>
+      <c r="F19" s="20"/>
       <c r="G19" s="9"/>
       <c r="H19" s="5"/>
     </row>
     <row r="20" ht="18.0" customHeight="1" outlineLevel="1">
-      <c r="A20" s="23" t="s">
-        <v>57</v>
-      </c>
-      <c r="B20" s="20" t="s">
-        <v>58</v>
-      </c>
-      <c r="C20" s="21">
-        <v>0.1</v>
-      </c>
-      <c r="D20" s="21">
-        <v>0.4</v>
-      </c>
-      <c r="E20" s="21">
-        <v>0.4</v>
-      </c>
-      <c r="F20" s="21">
-        <v>0.1</v>
-      </c>
+      <c r="A20" s="22" t="s">
+        <v>55</v>
+      </c>
+      <c r="B20" s="19" t="s">
+        <v>56</v>
+      </c>
+      <c r="C20" s="20"/>
+      <c r="D20" s="20"/>
+      <c r="E20" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="F20" s="20"/>
       <c r="G20" s="9"/>
       <c r="H20" s="9"/>
     </row>
     <row r="21" ht="18.0" customHeight="1" outlineLevel="1">
-      <c r="A21" s="23" t="s">
-        <v>59</v>
-      </c>
-      <c r="B21" s="20"/>
-      <c r="C21" s="21"/>
-      <c r="D21" s="21"/>
-      <c r="E21" s="21"/>
-      <c r="F21" s="21"/>
+      <c r="A21" s="22" t="s">
+        <v>57</v>
+      </c>
+      <c r="B21" s="19" t="s">
+        <v>58</v>
+      </c>
+      <c r="C21" s="20"/>
+      <c r="D21" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="E21" s="20"/>
+      <c r="F21" s="5" t="s">
+        <v>23</v>
+      </c>
       <c r="G21" s="9"/>
       <c r="H21" s="9"/>
     </row>
     <row r="22" ht="18.0" customHeight="1" outlineLevel="1">
-      <c r="A22" s="23" t="s">
+      <c r="A22" s="22" t="s">
+        <v>59</v>
+      </c>
+      <c r="B22" s="19" t="s">
         <v>60</v>
       </c>
-      <c r="B22" s="20"/>
-      <c r="C22" s="21"/>
-      <c r="D22" s="21"/>
-      <c r="E22" s="21"/>
-      <c r="F22" s="21"/>
+      <c r="C22" s="20"/>
+      <c r="D22" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="E22" s="20"/>
+      <c r="F22" s="5" t="s">
+        <v>31</v>
+      </c>
       <c r="G22" s="9"/>
       <c r="H22" s="9"/>
     </row>
     <row r="23" ht="18.0" customHeight="1" outlineLevel="1">
-      <c r="A23" s="23" t="s">
+      <c r="A23" s="22" t="s">
         <v>61</v>
       </c>
-      <c r="B23" s="20"/>
-      <c r="C23" s="21"/>
-      <c r="D23" s="21"/>
-      <c r="E23" s="21"/>
-      <c r="F23" s="21"/>
+      <c r="B23" s="19" t="s">
+        <v>62</v>
+      </c>
+      <c r="C23" s="20"/>
+      <c r="D23" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="E23" s="20"/>
+      <c r="F23" s="5" t="s">
+        <v>23</v>
+      </c>
       <c r="G23" s="9"/>
       <c r="H23" s="9"/>
     </row>
     <row r="24" ht="18.0" customHeight="1" outlineLevel="1">
-      <c r="A24" s="23" t="s">
+      <c r="A24" s="22" t="s">
+        <v>63</v>
+      </c>
+      <c r="B24" s="19" t="s">
         <v>62</v>
       </c>
-      <c r="B24" s="20"/>
-      <c r="C24" s="21"/>
-      <c r="D24" s="21"/>
-      <c r="E24" s="21"/>
-      <c r="F24" s="21"/>
+      <c r="C24" s="20"/>
+      <c r="D24" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="E24" s="20"/>
+      <c r="F24" s="5" t="s">
+        <v>23</v>
+      </c>
       <c r="G24" s="9"/>
       <c r="H24" s="9"/>
     </row>
     <row r="25" ht="18.0" customHeight="1" outlineLevel="1">
-      <c r="A25" s="23" t="s">
-        <v>63</v>
-      </c>
-      <c r="B25" s="20"/>
-      <c r="C25" s="21"/>
-      <c r="D25" s="21"/>
-      <c r="E25" s="21"/>
-      <c r="F25" s="21"/>
+      <c r="A25" s="22" t="s">
+        <v>64</v>
+      </c>
+      <c r="B25" s="19" t="s">
+        <v>65</v>
+      </c>
+      <c r="C25" s="20"/>
+      <c r="D25" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="E25" s="20"/>
+      <c r="F25" s="5" t="s">
+        <v>31</v>
+      </c>
       <c r="G25" s="9"/>
       <c r="H25" s="9"/>
     </row>
     <row r="26" ht="18.0" customHeight="1" outlineLevel="1">
-      <c r="A26" s="28" t="s">
-        <v>64</v>
-      </c>
-      <c r="B26" s="20"/>
-      <c r="C26" s="21"/>
-      <c r="D26" s="21"/>
-      <c r="E26" s="21"/>
-      <c r="F26" s="21"/>
+      <c r="A26" s="27" t="s">
+        <v>66</v>
+      </c>
+      <c r="B26" s="19" t="s">
+        <v>67</v>
+      </c>
+      <c r="C26" s="20"/>
+      <c r="D26" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="E26" s="20"/>
+      <c r="F26" s="5" t="s">
+        <v>23</v>
+      </c>
       <c r="G26" s="9"/>
       <c r="H26" s="5"/>
     </row>
     <row r="27" ht="18.0" customHeight="1" outlineLevel="1">
-      <c r="A27" s="28" t="s">
-        <v>65</v>
-      </c>
-      <c r="B27" s="20"/>
-      <c r="C27" s="21"/>
-      <c r="D27" s="21"/>
-      <c r="E27" s="21"/>
-      <c r="F27" s="21"/>
+      <c r="A27" s="27" t="s">
+        <v>68</v>
+      </c>
+      <c r="B27" s="19" t="s">
+        <v>69</v>
+      </c>
+      <c r="C27" s="20"/>
+      <c r="D27" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="E27" s="20"/>
+      <c r="F27" s="5" t="s">
+        <v>31</v>
+      </c>
       <c r="G27" s="9"/>
       <c r="H27" s="5"/>
     </row>
     <row r="28" ht="18.0" customHeight="1" outlineLevel="1">
-      <c r="A28" s="28" t="s">
-        <v>66</v>
-      </c>
-      <c r="B28" s="20"/>
-      <c r="C28" s="21"/>
-      <c r="D28" s="21"/>
-      <c r="E28" s="21"/>
-      <c r="F28" s="21"/>
+      <c r="A28" s="27" t="s">
+        <v>70</v>
+      </c>
+      <c r="B28" s="19" t="s">
+        <v>69</v>
+      </c>
+      <c r="C28" s="20"/>
+      <c r="D28" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="E28" s="20"/>
+      <c r="F28" s="5" t="s">
+        <v>31</v>
+      </c>
       <c r="G28" s="9"/>
       <c r="H28" s="5"/>
     </row>
     <row r="29" ht="18.0" customHeight="1" outlineLevel="1">
-      <c r="A29" s="28" t="s">
-        <v>67</v>
-      </c>
-      <c r="B29" s="20"/>
-      <c r="C29" s="21"/>
-      <c r="D29" s="21"/>
-      <c r="E29" s="21"/>
-      <c r="F29" s="21"/>
+      <c r="A29" s="27" t="s">
+        <v>71</v>
+      </c>
+      <c r="B29" s="19" t="s">
+        <v>72</v>
+      </c>
+      <c r="C29" s="20"/>
+      <c r="D29" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="E29" s="20"/>
+      <c r="F29" s="20"/>
       <c r="G29" s="9"/>
       <c r="H29" s="5"/>
     </row>
     <row r="30" ht="18.0" customHeight="1" outlineLevel="1">
-      <c r="A30" s="28" t="s">
-        <v>68</v>
-      </c>
-      <c r="B30" s="20"/>
-      <c r="C30" s="21"/>
-      <c r="D30" s="21"/>
-      <c r="E30" s="21"/>
-      <c r="F30" s="21"/>
+      <c r="A30" s="27" t="s">
+        <v>74</v>
+      </c>
+      <c r="B30" s="19" t="s">
+        <v>75</v>
+      </c>
+      <c r="C30" s="20"/>
+      <c r="D30" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="E30" s="20"/>
+      <c r="F30" s="5" t="s">
+        <v>31</v>
+      </c>
       <c r="G30" s="9"/>
       <c r="H30" s="5"/>
     </row>
     <row r="31" ht="27.75" customHeight="1" outlineLevel="1">
-      <c r="A31" s="29" t="s">
-        <v>69</v>
-      </c>
-      <c r="B31" s="20" t="s">
-        <v>70</v>
-      </c>
-      <c r="C31" s="21">
-        <v>0.2</v>
-      </c>
-      <c r="D31" s="21">
-        <v>0.6</v>
-      </c>
-      <c r="E31" s="21">
-        <v>0.05</v>
-      </c>
-      <c r="F31" s="21">
-        <v>0.15</v>
+      <c r="A31" s="28" t="s">
+        <v>76</v>
+      </c>
+      <c r="B31" s="19" t="s">
+        <v>77</v>
+      </c>
+      <c r="C31" s="20"/>
+      <c r="D31" s="20"/>
+      <c r="E31" s="20"/>
+      <c r="F31" s="5" t="s">
+        <v>78</v>
       </c>
       <c r="G31" s="9"/>
       <c r="H31" s="5"/>
     </row>
     <row r="32" ht="18.0" customHeight="1" outlineLevel="1">
-      <c r="A32" s="29" t="s">
-        <v>71</v>
-      </c>
-      <c r="B32" s="20" t="s">
-        <v>72</v>
-      </c>
-      <c r="C32" s="21">
-        <v>0.2</v>
-      </c>
-      <c r="D32" s="21">
-        <v>0.6</v>
-      </c>
-      <c r="E32" s="21">
-        <v>0.05</v>
-      </c>
-      <c r="F32" s="21">
-        <v>0.15</v>
+      <c r="A32" s="28" t="s">
+        <v>79</v>
+      </c>
+      <c r="B32" s="19" t="s">
+        <v>80</v>
+      </c>
+      <c r="C32" s="20"/>
+      <c r="D32" s="20"/>
+      <c r="E32" s="20"/>
+      <c r="F32" s="5" t="s">
+        <v>78</v>
       </c>
       <c r="G32" s="9"/>
       <c r="H32" s="5"/>
     </row>
-    <row r="33" ht="14.25" customHeight="1">
-      <c r="A33" s="13" t="s">
+    <row r="33" ht="18.0" customHeight="1" outlineLevel="1">
+      <c r="A33" s="28" t="s">
+        <v>81</v>
+      </c>
+      <c r="B33" s="19"/>
+      <c r="C33" s="5"/>
+      <c r="D33" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="E33" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="F33" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="G33" s="9"/>
+      <c r="H33" s="5"/>
+    </row>
+    <row r="34" ht="18.0" customHeight="1" outlineLevel="1">
+      <c r="A34" s="28"/>
+      <c r="B34" s="19"/>
+      <c r="C34" s="20"/>
+      <c r="D34" s="20"/>
+      <c r="E34" s="20"/>
+      <c r="F34" s="20"/>
+      <c r="G34" s="9"/>
+      <c r="H34" s="5"/>
+    </row>
+    <row r="35" ht="14.25" customHeight="1">
+      <c r="A35" s="12" t="s">
+        <v>84</v>
+      </c>
+      <c r="B35" s="12"/>
+      <c r="C35" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="D35" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="E35" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="F35" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="G35" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="H35" s="14" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="36" ht="14.25" customHeight="1">
+      <c r="A36" s="29" t="s">
+        <v>85</v>
+      </c>
+      <c r="B36" s="19" t="s">
+        <v>86</v>
+      </c>
+      <c r="C36" s="19"/>
+      <c r="D36" s="19"/>
+      <c r="E36" s="4"/>
+      <c r="F36" s="19" t="s">
+        <v>78</v>
+      </c>
+      <c r="G36" s="4"/>
+      <c r="H36" s="30"/>
+    </row>
+    <row r="37" ht="14.25" customHeight="1" outlineLevel="1">
+      <c r="A37" s="29" t="s">
+        <v>87</v>
+      </c>
+      <c r="B37" s="19" t="s">
+        <v>88</v>
+      </c>
+      <c r="C37" s="19"/>
+      <c r="D37" s="19"/>
+      <c r="E37" s="4"/>
+      <c r="F37" s="19" t="s">
         <v>73</v>
       </c>
-      <c r="B33" s="13"/>
-      <c r="C33" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="D33" s="14" t="s">
-        <v>8</v>
-      </c>
-      <c r="E33" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="F33" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="G33" s="14" t="s">
-        <v>11</v>
-      </c>
-      <c r="H33" s="15" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="34" ht="14.25" customHeight="1">
-      <c r="A34" s="30" t="s">
-        <v>74</v>
-      </c>
-      <c r="B34" s="20" t="s">
-        <v>75</v>
-      </c>
-      <c r="C34" s="31">
-        <v>0.15</v>
-      </c>
-      <c r="D34" s="4"/>
-      <c r="E34" s="4"/>
-      <c r="F34" s="31">
-        <v>0.7</v>
-      </c>
-      <c r="G34" s="4"/>
-      <c r="H34" s="31">
-        <v>0.15</v>
-      </c>
-    </row>
-    <row r="35" ht="14.25" customHeight="1" outlineLevel="1">
-      <c r="A35" s="30" t="s">
-        <v>76</v>
-      </c>
-      <c r="B35" s="20" t="s">
-        <v>77</v>
-      </c>
-      <c r="C35" s="31">
-        <v>0.15</v>
-      </c>
-      <c r="D35" s="20"/>
-      <c r="E35" s="4"/>
-      <c r="F35" s="31">
-        <v>0.7</v>
-      </c>
-      <c r="G35" s="4"/>
-      <c r="H35" s="31">
-        <v>0.15</v>
-      </c>
-    </row>
-    <row r="36" ht="14.25" customHeight="1" outlineLevel="1">
-      <c r="A36" s="30" t="s">
+      <c r="G37" s="4"/>
+      <c r="H37" s="30"/>
+    </row>
+    <row r="38" ht="14.25" customHeight="1" outlineLevel="1">
+      <c r="A38" s="31" t="s">
+        <v>89</v>
+      </c>
+      <c r="B38" s="19" t="s">
+        <v>90</v>
+      </c>
+      <c r="C38" s="19"/>
+      <c r="D38" s="19"/>
+      <c r="E38" s="4"/>
+      <c r="F38" s="19" t="s">
         <v>78</v>
       </c>
-      <c r="B36" s="20" t="s">
-        <v>79</v>
-      </c>
-      <c r="C36" s="31">
-        <v>0.15</v>
-      </c>
-      <c r="D36" s="4"/>
-      <c r="E36" s="4"/>
-      <c r="F36" s="31">
-        <v>0.7</v>
-      </c>
-      <c r="G36" s="4"/>
-      <c r="H36" s="31">
-        <v>0.15</v>
-      </c>
-    </row>
-    <row r="37" ht="14.25" customHeight="1" outlineLevel="1">
-      <c r="A37" s="4"/>
-      <c r="B37" s="4"/>
-      <c r="C37" s="4"/>
-      <c r="D37" s="4"/>
-      <c r="E37" s="4"/>
-      <c r="F37" s="4"/>
-      <c r="G37" s="4"/>
-      <c r="H37" s="4"/>
-    </row>
-    <row r="38" ht="14.25" customHeight="1" outlineLevel="1">
-      <c r="A38" s="13" t="s">
-        <v>80</v>
-      </c>
-      <c r="B38" s="13"/>
-      <c r="C38" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="D38" s="14" t="s">
-        <v>8</v>
-      </c>
-      <c r="E38" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="F38" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="G38" s="14" t="s">
-        <v>11</v>
-      </c>
-      <c r="H38" s="15" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="39" ht="14.25" customHeight="1">
-      <c r="A39" s="30" t="s">
-        <v>81</v>
-      </c>
-      <c r="B39" s="20" t="s">
-        <v>82</v>
-      </c>
-      <c r="C39" s="31">
-        <v>0.3</v>
-      </c>
-      <c r="D39" s="31">
-        <v>0.5</v>
-      </c>
+      <c r="G38" s="4"/>
+      <c r="H38" s="30"/>
+    </row>
+    <row r="39" ht="14.25" customHeight="1" outlineLevel="1">
+      <c r="A39" s="29" t="s">
+        <v>91</v>
+      </c>
+      <c r="B39" s="19" t="s">
+        <v>92</v>
+      </c>
+      <c r="C39" s="30"/>
+      <c r="D39" s="4"/>
       <c r="E39" s="4"/>
-      <c r="F39" s="31">
-        <v>0.2</v>
+      <c r="F39" s="19" t="s">
+        <v>31</v>
       </c>
       <c r="G39" s="4"/>
-      <c r="H39" s="4"/>
+      <c r="H39" s="30"/>
     </row>
     <row r="40" ht="14.25" customHeight="1" outlineLevel="1">
-      <c r="A40" s="30" t="s">
-        <v>83</v>
-      </c>
-      <c r="B40" s="20" t="s">
-        <v>84</v>
-      </c>
+      <c r="A40" s="19" t="s">
+        <v>93</v>
+      </c>
+      <c r="B40" s="4"/>
       <c r="C40" s="4"/>
       <c r="D40" s="4"/>
       <c r="E40" s="4"/>
-      <c r="F40" s="31">
-        <v>0.4</v>
+      <c r="F40" s="19" t="s">
+        <v>94</v>
       </c>
       <c r="G40" s="4"/>
-      <c r="H40" s="31">
-        <v>0.6</v>
-      </c>
+      <c r="H40" s="4"/>
     </row>
     <row r="41" ht="14.25" customHeight="1" outlineLevel="1">
-      <c r="A41" s="30" t="s">
-        <v>85</v>
-      </c>
-      <c r="B41" s="20" t="s">
-        <v>86</v>
-      </c>
+      <c r="A41" s="4"/>
+      <c r="B41" s="4"/>
       <c r="C41" s="4"/>
       <c r="D41" s="4"/>
       <c r="E41" s="4"/>
-      <c r="F41" s="31">
-        <v>0.4</v>
-      </c>
+      <c r="F41" s="4"/>
       <c r="G41" s="4"/>
-      <c r="H41" s="31">
-        <v>0.6</v>
-      </c>
+      <c r="H41" s="4"/>
     </row>
     <row r="42" ht="14.25" customHeight="1" outlineLevel="1">
-      <c r="A42" s="30" t="s">
-        <v>87</v>
-      </c>
-      <c r="B42" s="20" t="s">
-        <v>88</v>
-      </c>
-      <c r="C42" s="31">
-        <v>0.4</v>
-      </c>
-      <c r="D42" s="4"/>
-      <c r="E42" s="4"/>
-      <c r="F42" s="31"/>
-      <c r="G42" s="4"/>
-      <c r="H42" s="31">
-        <v>0.6</v>
-      </c>
-    </row>
-    <row r="43" ht="14.25" customHeight="1" outlineLevel="1">
-      <c r="A43" s="20" t="s">
-        <v>89</v>
-      </c>
-      <c r="B43" s="20" t="s">
-        <v>90</v>
-      </c>
-      <c r="C43" s="31">
-        <v>1.0</v>
-      </c>
-      <c r="D43" s="31">
-        <v>1.0</v>
-      </c>
-      <c r="E43" s="31">
-        <v>1.0</v>
-      </c>
-      <c r="F43" s="31">
-        <v>1.0</v>
-      </c>
-      <c r="G43" s="31">
-        <v>1.0</v>
-      </c>
-      <c r="H43" s="31">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="44" ht="14.25" customHeight="1">
-      <c r="A44" s="4"/>
-      <c r="B44" s="4"/>
+      <c r="A42" s="12" t="s">
+        <v>95</v>
+      </c>
+      <c r="B42" s="12"/>
+      <c r="C42" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="D42" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="E42" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="F42" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="G42" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="H42" s="14" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="43" ht="14.25" customHeight="1">
+      <c r="A43" s="29" t="s">
+        <v>96</v>
+      </c>
+      <c r="B43" s="19"/>
+      <c r="C43" s="30"/>
+      <c r="D43" s="19" t="s">
+        <v>17</v>
+      </c>
+      <c r="E43" s="4"/>
+      <c r="F43" s="30"/>
+      <c r="G43" s="4"/>
+      <c r="H43" s="19"/>
+    </row>
+    <row r="44" ht="14.25" customHeight="1" outlineLevel="1">
+      <c r="A44" s="29" t="s">
+        <v>97</v>
+      </c>
+      <c r="B44" s="19"/>
       <c r="C44" s="4"/>
-      <c r="D44" s="4"/>
-      <c r="E44" s="4"/>
-      <c r="F44" s="4"/>
+      <c r="D44" s="19" t="s">
+        <v>31</v>
+      </c>
+      <c r="E44" s="19" t="s">
+        <v>31</v>
+      </c>
+      <c r="F44" s="19" t="s">
+        <v>31</v>
+      </c>
       <c r="G44" s="4"/>
-      <c r="H44" s="4"/>
-    </row>
-    <row r="45" ht="14.25" customHeight="1">
-      <c r="A45" s="4"/>
-      <c r="B45" s="4"/>
+      <c r="H44" s="30"/>
+    </row>
+    <row r="45" ht="14.25" customHeight="1" outlineLevel="1">
+      <c r="A45" s="29" t="s">
+        <v>98</v>
+      </c>
+      <c r="B45" s="19"/>
       <c r="C45" s="4"/>
-      <c r="D45" s="4"/>
+      <c r="D45" s="19" t="s">
+        <v>47</v>
+      </c>
       <c r="E45" s="4"/>
-      <c r="F45" s="4"/>
+      <c r="F45" s="30"/>
       <c r="G45" s="4"/>
-      <c r="H45" s="4"/>
-    </row>
-    <row r="46" ht="14.25" customHeight="1"/>
-    <row r="47" ht="14.25" customHeight="1"/>
-    <row r="48" ht="14.25" customHeight="1"/>
-    <row r="49" ht="14.25" customHeight="1"/>
+      <c r="H45" s="30"/>
+    </row>
+    <row r="46" ht="14.25" customHeight="1" outlineLevel="1">
+      <c r="A46" s="29" t="s">
+        <v>99</v>
+      </c>
+      <c r="B46" s="19"/>
+      <c r="C46" s="30"/>
+      <c r="D46" s="4"/>
+      <c r="E46" s="4"/>
+      <c r="F46" s="30"/>
+      <c r="G46" s="4"/>
+      <c r="H46" s="19" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="47" ht="14.25" customHeight="1" outlineLevel="1">
+      <c r="A47" s="19" t="s">
+        <v>100</v>
+      </c>
+      <c r="B47" s="19"/>
+      <c r="C47" s="19" t="s">
+        <v>78</v>
+      </c>
+      <c r="D47" s="19" t="s">
+        <v>78</v>
+      </c>
+      <c r="E47" s="19" t="s">
+        <v>78</v>
+      </c>
+      <c r="F47" s="19" t="s">
+        <v>78</v>
+      </c>
+      <c r="G47" s="19" t="s">
+        <v>78</v>
+      </c>
+      <c r="H47" s="19" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="48" ht="14.25" customHeight="1">
+      <c r="A48" s="19" t="s">
+        <v>101</v>
+      </c>
+      <c r="B48" s="19"/>
+      <c r="C48" s="19" t="s">
+        <v>78</v>
+      </c>
+      <c r="D48" s="19" t="s">
+        <v>102</v>
+      </c>
+      <c r="E48" s="19" t="s">
+        <v>47</v>
+      </c>
+      <c r="F48" s="19" t="s">
+        <v>47</v>
+      </c>
+      <c r="G48" s="19" t="s">
+        <v>78</v>
+      </c>
+      <c r="H48" s="19" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="49" ht="14.25" customHeight="1">
+      <c r="A49" s="4"/>
+      <c r="B49" s="4"/>
+      <c r="C49" s="4"/>
+      <c r="D49" s="4"/>
+      <c r="E49" s="4"/>
+      <c r="F49" s="4"/>
+      <c r="G49" s="4"/>
+      <c r="H49" s="4"/>
+    </row>
     <row r="50" ht="14.25" customHeight="1"/>
     <row r="51" ht="14.25" customHeight="1"/>
     <row r="52" ht="14.25" customHeight="1"/>
@@ -2728,11 +2848,15 @@
     <row r="984" ht="14.25" customHeight="1"/>
     <row r="985" ht="14.25" customHeight="1"/>
     <row r="986" ht="14.25" customHeight="1"/>
+    <row r="987" ht="14.25" customHeight="1"/>
+    <row r="988" ht="14.25" customHeight="1"/>
+    <row r="989" ht="14.25" customHeight="1"/>
+    <row r="990" ht="14.25" customHeight="1"/>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="A2:D2"/>
     <mergeCell ref="C4:G4"/>
-    <mergeCell ref="J4:K4"/>
+    <mergeCell ref="L4:M4"/>
   </mergeCells>
   <printOptions/>
   <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>
@@ -2767,788 +2891,1103 @@
   <sheetData>
     <row r="1" ht="14.25" customHeight="1"/>
     <row r="2" ht="14.25" customHeight="1">
-      <c r="A2" s="16" t="s">
-        <v>91</v>
-      </c>
-      <c r="B2" s="16" t="s">
-        <v>92</v>
-      </c>
-      <c r="C2" s="16" t="s">
-        <v>93</v>
-      </c>
-      <c r="D2" s="14" t="s">
-        <v>94</v>
-      </c>
-      <c r="E2" s="16" t="s">
-        <v>95</v>
-      </c>
-      <c r="F2" s="16" t="s">
-        <v>96</v>
+      <c r="A2" s="15" t="s">
+        <v>104</v>
+      </c>
+      <c r="B2" s="15" t="s">
+        <v>105</v>
+      </c>
+      <c r="C2" s="15" t="s">
+        <v>106</v>
+      </c>
+      <c r="D2" s="13" t="s">
+        <v>107</v>
+      </c>
+      <c r="E2" s="15" t="s">
+        <v>108</v>
+      </c>
+      <c r="F2" s="15" t="s">
+        <v>109</v>
       </c>
       <c r="H2" s="32" t="s">
-        <v>97</v>
+        <v>110</v>
       </c>
       <c r="I2" s="33"/>
       <c r="J2" s="33"/>
       <c r="K2" s="34"/>
+      <c r="L2" s="35" t="s">
+        <v>111</v>
+      </c>
+      <c r="M2" s="33"/>
+      <c r="N2" s="33"/>
+      <c r="O2" s="34"/>
     </row>
     <row r="3" ht="14.25" customHeight="1">
       <c r="A3" s="4" t="s">
-        <v>98</v>
+        <v>112</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3" s="4"/>
-      <c r="D3" s="4"/>
-      <c r="E3" s="35">
-        <v>0.0</v>
-      </c>
-      <c r="F3" s="36">
-        <f t="shared" ref="F3:F7" si="1">D3*E3</f>
-        <v>0</v>
-      </c>
-      <c r="H3" s="16" t="s">
-        <v>92</v>
-      </c>
-      <c r="I3" s="16" t="s">
-        <v>93</v>
-      </c>
-      <c r="J3" s="16" t="s">
-        <v>99</v>
+        <v>6</v>
+      </c>
+      <c r="C3" s="19" t="s">
+        <v>113</v>
+      </c>
+      <c r="D3" s="19">
+        <v>10416.0</v>
+      </c>
+      <c r="E3" s="36">
+        <v>18.0</v>
+      </c>
+      <c r="F3" s="37">
+        <f t="shared" ref="F3:F8" si="1">D3*E3</f>
+        <v>187488</v>
+      </c>
+      <c r="H3" s="15" t="s">
+        <v>105</v>
+      </c>
+      <c r="I3" s="15" t="s">
+        <v>106</v>
+      </c>
+      <c r="J3" s="15" t="s">
+        <v>114</v>
       </c>
       <c r="K3" s="16" t="s">
-        <v>100</v>
+        <v>115</v>
+      </c>
+      <c r="L3" s="16" t="s">
+        <v>116</v>
+      </c>
+      <c r="M3" s="16" t="s">
+        <v>117</v>
+      </c>
+      <c r="N3" s="16" t="s">
+        <v>118</v>
+      </c>
+      <c r="O3" s="16" t="s">
+        <v>119</v>
       </c>
     </row>
     <row r="4" ht="14.25" customHeight="1">
       <c r="A4" s="4" t="s">
-        <v>101</v>
+        <v>120</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C4" s="37"/>
-      <c r="D4" s="4"/>
-      <c r="E4" s="35">
-        <v>0.0</v>
-      </c>
-      <c r="F4" s="36">
+        <v>7</v>
+      </c>
+      <c r="C4" s="23" t="s">
+        <v>113</v>
+      </c>
+      <c r="D4" s="19">
+        <v>7689.0</v>
+      </c>
+      <c r="E4" s="36">
+        <v>2.0</v>
+      </c>
+      <c r="F4" s="37">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>15378</v>
       </c>
       <c r="H4" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="I4" s="4"/>
-      <c r="J4" s="4"/>
-      <c r="K4" s="4"/>
+        <v>6</v>
+      </c>
+      <c r="I4" s="19" t="s">
+        <v>113</v>
+      </c>
+      <c r="J4" s="19">
+        <v>10416.0</v>
+      </c>
+      <c r="K4" s="38">
+        <v>187488.0</v>
+      </c>
+      <c r="L4" s="39"/>
+      <c r="M4" s="39"/>
+      <c r="N4" s="39"/>
+      <c r="O4" s="39">
+        <f>6*10416</f>
+        <v>62496</v>
+      </c>
     </row>
     <row r="5" ht="14.25" customHeight="1">
       <c r="A5" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>102</v>
-      </c>
-      <c r="C5" s="4"/>
-      <c r="D5" s="4"/>
-      <c r="E5" s="35">
-        <v>0.0</v>
-      </c>
-      <c r="F5" s="36">
+        <v>121</v>
+      </c>
+      <c r="C5" s="19" t="s">
+        <v>25</v>
+      </c>
+      <c r="D5" s="19">
+        <v>7500.0</v>
+      </c>
+      <c r="E5" s="36">
+        <v>2.0</v>
+      </c>
+      <c r="F5" s="37">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>15000</v>
       </c>
       <c r="H5" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="I5" s="37"/>
-      <c r="J5" s="4"/>
-      <c r="K5" s="4"/>
+        <v>7</v>
+      </c>
+      <c r="I5" s="23" t="s">
+        <v>113</v>
+      </c>
+      <c r="J5" s="19">
+        <v>7689.0</v>
+      </c>
+      <c r="K5" s="38">
+        <v>15378.0</v>
+      </c>
+      <c r="L5" s="40">
+        <f>24*7689</f>
+        <v>184536</v>
+      </c>
+      <c r="M5" s="40">
+        <f>32*7689</f>
+        <v>246048</v>
+      </c>
+      <c r="N5" s="40">
+        <f>8*7689</f>
+        <v>61512</v>
+      </c>
+      <c r="O5" s="39">
+        <f>6*7689</f>
+        <v>46134</v>
+      </c>
     </row>
     <row r="6" ht="14.25" customHeight="1">
       <c r="A6" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>122</v>
+      </c>
+      <c r="C6" s="19" t="s">
+        <v>123</v>
+      </c>
+      <c r="D6" s="19">
+        <v>6666.0</v>
+      </c>
+      <c r="E6" s="36">
+        <v>2.0</v>
+      </c>
+      <c r="F6" s="37">
+        <f t="shared" si="1"/>
+        <v>13332</v>
+      </c>
+      <c r="H6" s="4" t="s">
+        <v>124</v>
+      </c>
+      <c r="I6" s="19" t="s">
+        <v>25</v>
+      </c>
+      <c r="J6" s="19">
+        <v>7500.0</v>
+      </c>
+      <c r="K6" s="38">
+        <v>15000.0</v>
+      </c>
+      <c r="L6" s="40">
+        <f>8*7500</f>
+        <v>60000</v>
+      </c>
+      <c r="M6" s="39"/>
+      <c r="N6" s="39"/>
+      <c r="O6" s="39">
+        <f>6*7500</f>
+        <v>45000</v>
+      </c>
+    </row>
+    <row r="7" ht="14.25" customHeight="1">
+      <c r="A7" s="19" t="s">
+        <v>125</v>
+      </c>
+      <c r="B7" s="19" t="s">
+        <v>126</v>
+      </c>
+      <c r="C7" s="19" t="s">
+        <v>25</v>
+      </c>
+      <c r="D7" s="19">
+        <v>7852.0</v>
+      </c>
+      <c r="E7" s="36">
+        <v>2.0</v>
+      </c>
+      <c r="F7" s="37">
+        <f t="shared" si="1"/>
+        <v>15704</v>
+      </c>
+      <c r="H7" s="4" t="s">
+        <v>122</v>
+      </c>
+      <c r="I7" s="19" t="s">
+        <v>123</v>
+      </c>
+      <c r="J7" s="19">
+        <v>6666.0</v>
+      </c>
+      <c r="K7" s="38">
+        <v>13332.0</v>
+      </c>
+      <c r="L7" s="40">
+        <f>6*6666</f>
+        <v>39996</v>
+      </c>
+      <c r="M7" s="40">
+        <f>18*6666</f>
+        <v>119988</v>
+      </c>
+      <c r="N7" s="40">
+        <f>40*666</f>
+        <v>26640</v>
+      </c>
+      <c r="O7" s="39">
+        <f>6*6666</f>
+        <v>39996</v>
+      </c>
+    </row>
+    <row r="8" ht="14.25" customHeight="1">
+      <c r="A8" s="19" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8" s="19" t="s">
+        <v>127</v>
+      </c>
+      <c r="C8" s="19" t="s">
+        <v>123</v>
+      </c>
+      <c r="D8" s="19">
+        <v>14583.0</v>
+      </c>
+      <c r="E8" s="36">
+        <v>14.0</v>
+      </c>
+      <c r="F8" s="37">
+        <f t="shared" si="1"/>
+        <v>204162</v>
+      </c>
+      <c r="H8" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="4" t="s">
-        <v>103</v>
-      </c>
-      <c r="C6" s="4"/>
-      <c r="D6" s="4"/>
-      <c r="E6" s="35">
+      <c r="I8" s="19" t="s">
+        <v>25</v>
+      </c>
+      <c r="J8" s="19">
+        <v>7852.0</v>
+      </c>
+      <c r="K8" s="38">
+        <v>15704.0</v>
+      </c>
+      <c r="L8" s="40">
+        <f>22*7852</f>
+        <v>172744</v>
+      </c>
+      <c r="M8" s="39"/>
+      <c r="N8" s="39"/>
+      <c r="O8" s="39">
+        <f>6*15704</f>
+        <v>94224</v>
+      </c>
+    </row>
+    <row r="9" ht="14.25" customHeight="1">
+      <c r="A9" s="4"/>
+      <c r="B9" s="6" t="s">
+        <v>128</v>
+      </c>
+      <c r="C9" s="7"/>
+      <c r="D9" s="7"/>
+      <c r="E9" s="8"/>
+      <c r="F9" s="37">
+        <f>SUM(F3:F8)</f>
+        <v>451064</v>
+      </c>
+      <c r="H9" s="19" t="s">
+        <v>11</v>
+      </c>
+      <c r="I9" s="19" t="s">
+        <v>123</v>
+      </c>
+      <c r="J9" s="19">
+        <v>14583.0</v>
+      </c>
+      <c r="K9" s="38">
+        <v>204162.0</v>
+      </c>
+      <c r="L9" s="40">
         <v>0.0</v>
       </c>
-      <c r="F6" s="36">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="H6" s="4" t="s">
+      <c r="M9" s="39"/>
+      <c r="N9" s="39"/>
+      <c r="O9" s="39">
+        <f>32*14583</f>
+        <v>466656</v>
+      </c>
+    </row>
+    <row r="10" ht="14.25" customHeight="1"/>
+    <row r="11" ht="14.25" customHeight="1"/>
+    <row r="12" ht="14.25" customHeight="1">
+      <c r="A12" s="15" t="s">
         <v>104</v>
       </c>
-      <c r="I6" s="4"/>
-      <c r="J6" s="4"/>
-      <c r="K6" s="4"/>
-    </row>
-    <row r="7" ht="14.25" customHeight="1">
-      <c r="A7" s="4" t="s">
+      <c r="B12" s="15" t="s">
         <v>105</v>
       </c>
-      <c r="B7" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="C7" s="4"/>
-      <c r="D7" s="4"/>
-      <c r="E7" s="35">
-        <v>0.0</v>
-      </c>
-      <c r="F7" s="36">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="H7" s="4" t="s">
-        <v>103</v>
-      </c>
-      <c r="I7" s="4"/>
-      <c r="J7" s="4"/>
-      <c r="K7" s="4"/>
-    </row>
-    <row r="8" ht="14.25" customHeight="1">
-      <c r="A8" s="4"/>
-      <c r="B8" s="6" t="s">
+      <c r="C12" s="15" t="s">
         <v>106</v>
       </c>
-      <c r="C8" s="7"/>
-      <c r="D8" s="7"/>
-      <c r="E8" s="8"/>
-      <c r="F8" s="36">
-        <f>SUM(F3:F7)</f>
-        <v>0</v>
-      </c>
-      <c r="H8" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="I8" s="4"/>
-      <c r="J8" s="4"/>
-      <c r="K8" s="4"/>
-    </row>
-    <row r="9" ht="14.25" customHeight="1"/>
-    <row r="10" ht="14.25" customHeight="1"/>
-    <row r="11" ht="14.25" customHeight="1">
-      <c r="A11" s="16" t="s">
-        <v>91</v>
-      </c>
-      <c r="B11" s="16" t="s">
-        <v>92</v>
-      </c>
-      <c r="C11" s="16" t="s">
-        <v>93</v>
-      </c>
-      <c r="D11" s="14" t="s">
-        <v>107</v>
-      </c>
-      <c r="E11" s="16" t="s">
-        <v>95</v>
-      </c>
-      <c r="F11" s="16" t="s">
+      <c r="D12" s="13" t="s">
+        <v>129</v>
+      </c>
+      <c r="E12" s="15" t="s">
         <v>108</v>
       </c>
-      <c r="H11" s="32" t="s">
-        <v>109</v>
-      </c>
-      <c r="I11" s="34"/>
-    </row>
-    <row r="12" ht="14.25" customHeight="1">
-      <c r="A12" s="4" t="s">
-        <v>98</v>
-      </c>
-      <c r="B12" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C12" s="4"/>
-      <c r="D12" s="4"/>
-      <c r="E12" s="35">
-        <v>0.0</v>
-      </c>
-      <c r="F12" s="36">
-        <f t="shared" ref="F12:F16" si="2">D12*E12</f>
-        <v>0</v>
-      </c>
-      <c r="H12" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="I12" s="36">
-        <f t="shared" ref="I12:I16" si="3">F3+F12+F21+F30+F39</f>
-        <v>0</v>
-      </c>
+      <c r="F12" s="15" t="s">
+        <v>130</v>
+      </c>
+      <c r="H12" s="32" t="s">
+        <v>131</v>
+      </c>
+      <c r="I12" s="34"/>
     </row>
     <row r="13" ht="14.25" customHeight="1">
       <c r="A13" s="4" t="s">
-        <v>101</v>
+        <v>112</v>
       </c>
       <c r="B13" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C13" s="19" t="s">
+        <v>113</v>
+      </c>
+      <c r="D13" s="19">
+        <v>10416.0</v>
+      </c>
+      <c r="E13" s="36">
+        <v>4.0</v>
+      </c>
+      <c r="F13" s="37">
+        <f t="shared" ref="F13:F18" si="2">D13*E13</f>
+        <v>41664</v>
+      </c>
+      <c r="H13" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="I13" s="37">
+        <f t="shared" ref="I13:I18" si="3">F3+F13+F23+F33+F43</f>
+        <v>291648</v>
+      </c>
+    </row>
+    <row r="14" ht="14.25" customHeight="1">
+      <c r="A14" s="4" t="s">
+        <v>120</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C14" s="23" t="s">
+        <v>113</v>
+      </c>
+      <c r="D14" s="19">
+        <v>7689.0</v>
+      </c>
+      <c r="E14" s="36">
+        <v>14.0</v>
+      </c>
+      <c r="F14" s="37">
+        <f t="shared" si="2"/>
+        <v>107646</v>
+      </c>
+      <c r="H14" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="I14" s="37">
+        <f t="shared" si="3"/>
+        <v>891924</v>
+      </c>
+    </row>
+    <row r="15" ht="14.25" customHeight="1">
+      <c r="A15" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C13" s="37"/>
-      <c r="D13" s="4"/>
-      <c r="E13" s="35">
+      <c r="B15" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="C15" s="19" t="s">
+        <v>25</v>
+      </c>
+      <c r="D15" s="19">
+        <v>7500.0</v>
+      </c>
+      <c r="E15" s="41">
         <v>0.0</v>
       </c>
-      <c r="F13" s="36">
+      <c r="F15" s="37">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="H13" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="I13" s="36">
+      <c r="H15" s="4" t="s">
+        <v>124</v>
+      </c>
+      <c r="I15" s="37">
         <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" ht="14.25" customHeight="1">
-      <c r="A14" s="4" t="s">
+        <v>90000</v>
+      </c>
+    </row>
+    <row r="16" ht="14.25" customHeight="1">
+      <c r="A16" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B14" s="4" t="s">
-        <v>102</v>
-      </c>
-      <c r="C14" s="4"/>
-      <c r="D14" s="4"/>
-      <c r="E14" s="35">
+      <c r="B16" s="4" t="s">
+        <v>122</v>
+      </c>
+      <c r="C16" s="19" t="s">
+        <v>123</v>
+      </c>
+      <c r="D16" s="19">
+        <v>6666.0</v>
+      </c>
+      <c r="E16" s="41">
         <v>0.0</v>
       </c>
-      <c r="F14" s="36">
+      <c r="F16" s="37">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="H14" s="4" t="s">
+      <c r="H16" s="4" t="s">
+        <v>122</v>
+      </c>
+      <c r="I16" s="37">
+        <f t="shared" si="3"/>
+        <v>533280</v>
+      </c>
+    </row>
+    <row r="17" ht="14.25" customHeight="1">
+      <c r="A17" s="4" t="s">
+        <v>132</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C17" s="19" t="s">
+        <v>25</v>
+      </c>
+      <c r="D17" s="19">
+        <v>7852.0</v>
+      </c>
+      <c r="E17" s="36">
+        <v>44.0</v>
+      </c>
+      <c r="F17" s="37">
+        <f t="shared" si="2"/>
+        <v>345488</v>
+      </c>
+      <c r="H17" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="I17" s="37">
+        <f t="shared" si="3"/>
+        <v>408304</v>
+      </c>
+    </row>
+    <row r="18" ht="14.25" customHeight="1">
+      <c r="A18" s="19" t="s">
+        <v>133</v>
+      </c>
+      <c r="B18" s="19" t="s">
+        <v>127</v>
+      </c>
+      <c r="C18" s="19" t="s">
+        <v>123</v>
+      </c>
+      <c r="D18" s="19">
+        <v>14583.0</v>
+      </c>
+      <c r="E18" s="36">
+        <v>2.0</v>
+      </c>
+      <c r="F18" s="37">
+        <f t="shared" si="2"/>
+        <v>29166</v>
+      </c>
+      <c r="H18" s="19" t="s">
+        <v>133</v>
+      </c>
+      <c r="I18" s="37">
+        <f t="shared" si="3"/>
+        <v>466656</v>
+      </c>
+    </row>
+    <row r="19" ht="14.25" customHeight="1">
+      <c r="A19" s="4"/>
+      <c r="B19" s="6" t="s">
+        <v>134</v>
+      </c>
+      <c r="C19" s="7"/>
+      <c r="D19" s="7"/>
+      <c r="E19" s="8"/>
+      <c r="F19" s="37">
+        <f>SUM(F13:F17)</f>
+        <v>494798</v>
+      </c>
+      <c r="H19" s="42" t="s">
+        <v>135</v>
+      </c>
+      <c r="I19" s="43">
+        <f>SUM(I13:I17)</f>
+        <v>2215156</v>
+      </c>
+    </row>
+    <row r="20" ht="14.25" customHeight="1"/>
+    <row r="21" ht="14.25" customHeight="1"/>
+    <row r="22" ht="14.25" customHeight="1">
+      <c r="A22" s="15" t="s">
         <v>104</v>
       </c>
-      <c r="I14" s="36">
-        <f t="shared" si="3"/>
+      <c r="B22" s="15" t="s">
+        <v>105</v>
+      </c>
+      <c r="C22" s="15" t="s">
+        <v>106</v>
+      </c>
+      <c r="D22" s="13" t="s">
+        <v>129</v>
+      </c>
+      <c r="E22" s="15" t="s">
+        <v>108</v>
+      </c>
+      <c r="F22" s="15" t="s">
+        <v>136</v>
+      </c>
+      <c r="H22" s="32" t="s">
+        <v>137</v>
+      </c>
+      <c r="I22" s="34"/>
+    </row>
+    <row r="23" ht="14.25" customHeight="1">
+      <c r="A23" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="B23" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C23" s="19" t="s">
+        <v>113</v>
+      </c>
+      <c r="D23" s="19">
+        <v>10416.0</v>
+      </c>
+      <c r="E23" s="41">
+        <v>0.0</v>
+      </c>
+      <c r="F23" s="37">
+        <f t="shared" ref="F23:F28" si="4">D23*E23</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="15" ht="14.25" customHeight="1">
-      <c r="A15" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="B15" s="4" t="s">
-        <v>103</v>
-      </c>
-      <c r="C15" s="4"/>
-      <c r="D15" s="4"/>
-      <c r="E15" s="35">
+      <c r="H23" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="I23" s="37">
+        <f>F9</f>
+        <v>451064</v>
+      </c>
+    </row>
+    <row r="24" ht="14.25" customHeight="1">
+      <c r="A24" s="4" t="s">
+        <v>120</v>
+      </c>
+      <c r="B24" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C24" s="23" t="s">
+        <v>113</v>
+      </c>
+      <c r="D24" s="19">
+        <v>7689.0</v>
+      </c>
+      <c r="E24" s="36">
+        <v>64.0</v>
+      </c>
+      <c r="F24" s="37">
+        <f t="shared" si="4"/>
+        <v>492096</v>
+      </c>
+      <c r="H24" s="4" t="s">
+        <v>138</v>
+      </c>
+      <c r="I24" s="37">
+        <f>F19</f>
+        <v>494798</v>
+      </c>
+    </row>
+    <row r="25" ht="14.25" customHeight="1">
+      <c r="A25" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B25" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="C25" s="19" t="s">
+        <v>25</v>
+      </c>
+      <c r="D25" s="19">
+        <v>7500.0</v>
+      </c>
+      <c r="E25" s="41">
         <v>0.0</v>
       </c>
-      <c r="F15" s="36">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="H15" s="4" t="s">
-        <v>103</v>
-      </c>
-      <c r="I15" s="36">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" ht="14.25" customHeight="1">
-      <c r="A16" s="4" t="s">
-        <v>105</v>
-      </c>
-      <c r="B16" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="C16" s="4"/>
-      <c r="D16" s="4"/>
-      <c r="E16" s="35">
-        <v>0.0</v>
-      </c>
-      <c r="F16" s="36">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="H16" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="I16" s="36">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" ht="14.25" customHeight="1">
-      <c r="A17" s="4"/>
-      <c r="B17" s="6" t="s">
-        <v>110</v>
-      </c>
-      <c r="C17" s="7"/>
-      <c r="D17" s="7"/>
-      <c r="E17" s="8"/>
-      <c r="F17" s="36">
-        <f>SUM(F12:F16)</f>
-        <v>0</v>
-      </c>
-      <c r="H17" s="38" t="s">
-        <v>111</v>
-      </c>
-      <c r="I17" s="39">
-        <f>SUM(I12:I16)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" ht="14.25" customHeight="1"/>
-    <row r="19" ht="14.25" customHeight="1"/>
-    <row r="20" ht="14.25" customHeight="1">
-      <c r="A20" s="16" t="s">
-        <v>91</v>
-      </c>
-      <c r="B20" s="16" t="s">
-        <v>92</v>
-      </c>
-      <c r="C20" s="16" t="s">
-        <v>93</v>
-      </c>
-      <c r="D20" s="14" t="s">
-        <v>107</v>
-      </c>
-      <c r="E20" s="16" t="s">
-        <v>95</v>
-      </c>
-      <c r="F20" s="16" t="s">
-        <v>112</v>
-      </c>
-      <c r="H20" s="32" t="s">
-        <v>113</v>
-      </c>
-      <c r="I20" s="34"/>
-    </row>
-    <row r="21" ht="14.25" customHeight="1">
-      <c r="A21" s="4" t="s">
-        <v>98</v>
-      </c>
-      <c r="B21" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C21" s="4"/>
-      <c r="D21" s="4"/>
-      <c r="E21" s="35">
-        <v>0.0</v>
-      </c>
-      <c r="F21" s="36">
-        <f t="shared" ref="F21:F25" si="4">D21*E21</f>
-        <v>0</v>
-      </c>
-      <c r="H21" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="I21" s="36">
-        <f>F8</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" ht="14.25" customHeight="1">
-      <c r="A22" s="4" t="s">
-        <v>101</v>
-      </c>
-      <c r="B22" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C22" s="37"/>
-      <c r="D22" s="4"/>
-      <c r="E22" s="35">
-        <v>0.0</v>
-      </c>
-      <c r="F22" s="36">
+      <c r="F25" s="37">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="H22" s="4" t="s">
-        <v>114</v>
-      </c>
-      <c r="I22" s="36">
-        <f>F17</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" ht="14.25" customHeight="1">
-      <c r="A23" s="4" t="s">
+      <c r="H25" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="I25" s="37">
+        <f>F29</f>
+        <v>758736</v>
+      </c>
+    </row>
+    <row r="26" ht="14.25" customHeight="1">
+      <c r="A26" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B23" s="4" t="s">
-        <v>102</v>
-      </c>
-      <c r="C23" s="4"/>
-      <c r="D23" s="4"/>
-      <c r="E23" s="35">
+      <c r="B26" s="4" t="s">
+        <v>122</v>
+      </c>
+      <c r="C26" s="19" t="s">
+        <v>123</v>
+      </c>
+      <c r="D26" s="19">
+        <v>6666.0</v>
+      </c>
+      <c r="E26" s="36">
+        <v>40.0</v>
+      </c>
+      <c r="F26" s="37">
+        <f t="shared" si="4"/>
+        <v>266640</v>
+      </c>
+      <c r="H26" s="4" t="s">
+        <v>139</v>
+      </c>
+      <c r="I26" s="37">
+        <f>F39</f>
+        <v>294294</v>
+      </c>
+    </row>
+    <row r="27" ht="14.25" customHeight="1">
+      <c r="A27" s="4" t="s">
+        <v>132</v>
+      </c>
+      <c r="B27" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C27" s="19" t="s">
+        <v>25</v>
+      </c>
+      <c r="D27" s="19">
+        <v>7852.0</v>
+      </c>
+      <c r="E27" s="41">
         <v>0.0</v>
       </c>
-      <c r="F23" s="36">
+      <c r="F27" s="37">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="H23" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="I23" s="36">
-        <f>F26</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" ht="14.25" customHeight="1">
-      <c r="A24" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="B24" s="4" t="s">
-        <v>103</v>
-      </c>
-      <c r="C24" s="4"/>
-      <c r="D24" s="4"/>
-      <c r="E24" s="35">
-        <v>0.0</v>
-      </c>
-      <c r="F24" s="36">
+      <c r="H27" s="4" t="s">
+        <v>140</v>
+      </c>
+      <c r="I27" s="37">
+        <f>F49</f>
+        <v>653754</v>
+      </c>
+    </row>
+    <row r="28" ht="14.25" customHeight="1">
+      <c r="A28" s="19" t="s">
+        <v>133</v>
+      </c>
+      <c r="B28" s="19" t="s">
+        <v>127</v>
+      </c>
+      <c r="C28" s="19" t="s">
+        <v>141</v>
+      </c>
+      <c r="D28" s="19">
+        <v>14583.0</v>
+      </c>
+      <c r="E28" s="36"/>
+      <c r="F28" s="37">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="H24" s="4" t="s">
-        <v>115</v>
-      </c>
-      <c r="I24" s="36">
-        <f>F35</f>
+      <c r="H28" s="4"/>
+      <c r="I28" s="37"/>
+    </row>
+    <row r="29" ht="14.25" customHeight="1">
+      <c r="A29" s="4"/>
+      <c r="B29" s="6" t="s">
+        <v>142</v>
+      </c>
+      <c r="C29" s="7"/>
+      <c r="D29" s="7"/>
+      <c r="E29" s="8"/>
+      <c r="F29" s="37">
+        <f>SUM(F23:F27)</f>
+        <v>758736</v>
+      </c>
+      <c r="H29" s="42" t="s">
+        <v>143</v>
+      </c>
+      <c r="I29" s="43">
+        <f>SUM(I23:I27)</f>
+        <v>2652646</v>
+      </c>
+    </row>
+    <row r="30" ht="14.25" customHeight="1"/>
+    <row r="31" ht="14.25" customHeight="1"/>
+    <row r="32" ht="14.25" customHeight="1">
+      <c r="A32" s="15" t="s">
+        <v>104</v>
+      </c>
+      <c r="B32" s="15" t="s">
+        <v>105</v>
+      </c>
+      <c r="C32" s="15" t="s">
+        <v>106</v>
+      </c>
+      <c r="D32" s="13" t="s">
+        <v>129</v>
+      </c>
+      <c r="E32" s="15" t="s">
+        <v>108</v>
+      </c>
+      <c r="F32" s="15" t="s">
+        <v>144</v>
+      </c>
+      <c r="H32" s="15" t="s">
+        <v>145</v>
+      </c>
+      <c r="I32" s="44">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="33" ht="14.25" customHeight="1">
+      <c r="A33" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="B33" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C33" s="19" t="s">
+        <v>113</v>
+      </c>
+      <c r="D33" s="19">
+        <v>10416.0</v>
+      </c>
+      <c r="E33" s="41">
+        <v>0.0</v>
+      </c>
+      <c r="F33" s="37">
+        <f t="shared" ref="F33:F38" si="5">D33*E33</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="25" ht="14.25" customHeight="1">
-      <c r="A25" s="4" t="s">
-        <v>105</v>
-      </c>
-      <c r="B25" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="C25" s="4"/>
-      <c r="D25" s="4"/>
-      <c r="E25" s="35">
+      <c r="H33" s="4" t="s">
+        <v>146</v>
+      </c>
+      <c r="I33" s="37">
+        <f>I29*I32</f>
+        <v>1591587.6</v>
+      </c>
+    </row>
+    <row r="34" ht="14.25" customHeight="1">
+      <c r="A34" s="4" t="s">
+        <v>120</v>
+      </c>
+      <c r="B34" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C34" s="23" t="s">
+        <v>113</v>
+      </c>
+      <c r="D34" s="19">
+        <v>7689.0</v>
+      </c>
+      <c r="E34" s="36">
+        <v>14.0</v>
+      </c>
+      <c r="F34" s="37">
+        <f t="shared" si="5"/>
+        <v>107646</v>
+      </c>
+      <c r="H34" s="4" t="s">
+        <v>147</v>
+      </c>
+      <c r="I34" s="37">
+        <f>I29+I33</f>
+        <v>4244233.6</v>
+      </c>
+    </row>
+    <row r="35" ht="14.25" customHeight="1">
+      <c r="A35" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B35" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="C35" s="19" t="s">
+        <v>25</v>
+      </c>
+      <c r="D35" s="19">
+        <v>7500.0</v>
+      </c>
+      <c r="E35" s="41">
         <v>0.0</v>
       </c>
-      <c r="F25" s="36">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="H25" s="4" t="s">
-        <v>116</v>
-      </c>
-      <c r="I25" s="36">
-        <f>F44</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" ht="14.25" customHeight="1">
-      <c r="A26" s="4"/>
-      <c r="B26" s="6" t="s">
-        <v>117</v>
-      </c>
-      <c r="C26" s="7"/>
-      <c r="D26" s="7"/>
-      <c r="E26" s="8"/>
-      <c r="F26" s="36">
-        <f>SUM(F21:F25)</f>
-        <v>0</v>
-      </c>
-      <c r="H26" s="38" t="s">
-        <v>118</v>
-      </c>
-      <c r="I26" s="39">
-        <f>SUM(I21:I25)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" ht="14.25" customHeight="1"/>
-    <row r="28" ht="14.25" customHeight="1"/>
-    <row r="29" ht="14.25" customHeight="1">
-      <c r="A29" s="16" t="s">
-        <v>91</v>
-      </c>
-      <c r="B29" s="16" t="s">
-        <v>92</v>
-      </c>
-      <c r="C29" s="16" t="s">
-        <v>93</v>
-      </c>
-      <c r="D29" s="14" t="s">
-        <v>107</v>
-      </c>
-      <c r="E29" s="16" t="s">
-        <v>95</v>
-      </c>
-      <c r="F29" s="16" t="s">
-        <v>119</v>
-      </c>
-      <c r="H29" s="16" t="s">
-        <v>120</v>
-      </c>
-      <c r="I29" s="40">
-        <v>0.6</v>
-      </c>
-    </row>
-    <row r="30" ht="14.25" customHeight="1">
-      <c r="A30" s="4" t="s">
-        <v>98</v>
-      </c>
-      <c r="B30" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C30" s="4" t="s">
-        <v>121</v>
-      </c>
-      <c r="D30" s="4"/>
-      <c r="E30" s="35">
-        <v>0.0</v>
-      </c>
-      <c r="F30" s="36">
-        <f t="shared" ref="F30:F34" si="5">D30*E30</f>
-        <v>0</v>
-      </c>
-      <c r="H30" s="4" t="s">
-        <v>122</v>
-      </c>
-      <c r="I30" s="36">
-        <f>I26*I29</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="31" ht="14.25" customHeight="1">
-      <c r="A31" s="4" t="s">
-        <v>101</v>
-      </c>
-      <c r="B31" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C31" s="37" t="s">
-        <v>123</v>
-      </c>
-      <c r="D31" s="4"/>
-      <c r="E31" s="35">
-        <v>0.0</v>
-      </c>
-      <c r="F31" s="36">
+      <c r="F35" s="37">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="H31" s="4" t="s">
-        <v>124</v>
-      </c>
-      <c r="I31" s="36">
-        <f>I26+I30</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="32" ht="14.25" customHeight="1">
-      <c r="A32" s="4" t="s">
+    </row>
+    <row r="36" ht="14.25" customHeight="1">
+      <c r="A36" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B32" s="4" t="s">
-        <v>102</v>
-      </c>
-      <c r="C32" s="4" t="s">
-        <v>125</v>
-      </c>
-      <c r="D32" s="4"/>
-      <c r="E32" s="35">
+      <c r="B36" s="4" t="s">
+        <v>122</v>
+      </c>
+      <c r="C36" s="19" t="s">
+        <v>123</v>
+      </c>
+      <c r="D36" s="19">
+        <v>6666.0</v>
+      </c>
+      <c r="E36" s="36">
+        <v>28.0</v>
+      </c>
+      <c r="F36" s="37">
+        <f t="shared" si="5"/>
+        <v>186648</v>
+      </c>
+    </row>
+    <row r="37" ht="14.25" customHeight="1">
+      <c r="A37" s="4" t="s">
+        <v>132</v>
+      </c>
+      <c r="B37" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C37" s="19" t="s">
+        <v>25</v>
+      </c>
+      <c r="D37" s="19">
+        <v>7852.0</v>
+      </c>
+      <c r="E37" s="41">
         <v>0.0</v>
       </c>
-      <c r="F32" s="36">
+      <c r="F37" s="37">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
-    <row r="33" ht="14.25" customHeight="1">
-      <c r="A33" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="B33" s="4" t="s">
-        <v>103</v>
-      </c>
-      <c r="C33" s="4" t="s">
-        <v>126</v>
-      </c>
-      <c r="D33" s="4"/>
-      <c r="E33" s="35">
+    <row r="38" ht="14.25" customHeight="1">
+      <c r="A38" s="19" t="s">
+        <v>133</v>
+      </c>
+      <c r="B38" s="19" t="s">
+        <v>127</v>
+      </c>
+      <c r="C38" s="19" t="s">
+        <v>123</v>
+      </c>
+      <c r="D38" s="19">
+        <v>14583.0</v>
+      </c>
+      <c r="E38" s="36">
         <v>0.0</v>
       </c>
-      <c r="F33" s="36">
+      <c r="F38" s="37">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
-    <row r="34" ht="14.25" customHeight="1">
-      <c r="A34" s="4" t="s">
+    <row r="39" ht="14.25" customHeight="1">
+      <c r="A39" s="4"/>
+      <c r="B39" s="6" t="s">
+        <v>148</v>
+      </c>
+      <c r="C39" s="7"/>
+      <c r="D39" s="7"/>
+      <c r="E39" s="8"/>
+      <c r="F39" s="37">
+        <f>SUM(F33:F37)</f>
+        <v>294294</v>
+      </c>
+    </row>
+    <row r="40" ht="14.25" customHeight="1"/>
+    <row r="41" ht="14.25" customHeight="1"/>
+    <row r="42" ht="14.25" customHeight="1">
+      <c r="A42" s="15" t="s">
+        <v>104</v>
+      </c>
+      <c r="B42" s="15" t="s">
         <v>105</v>
       </c>
-      <c r="B34" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="C34" s="4" t="s">
-        <v>126</v>
-      </c>
-      <c r="D34" s="4"/>
-      <c r="E34" s="35">
-        <v>0.0</v>
-      </c>
-      <c r="F34" s="36">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="35" ht="14.25" customHeight="1">
-      <c r="A35" s="4"/>
-      <c r="B35" s="6" t="s">
-        <v>127</v>
-      </c>
-      <c r="C35" s="7"/>
-      <c r="D35" s="7"/>
-      <c r="E35" s="8"/>
-      <c r="F35" s="36">
-        <f>SUM(F30:F34)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="36" ht="14.25" customHeight="1"/>
-    <row r="37" ht="14.25" customHeight="1"/>
-    <row r="38" ht="14.25" customHeight="1">
-      <c r="A38" s="16" t="s">
-        <v>91</v>
-      </c>
-      <c r="B38" s="16" t="s">
-        <v>92</v>
-      </c>
-      <c r="C38" s="16" t="s">
-        <v>93</v>
-      </c>
-      <c r="D38" s="14" t="s">
-        <v>107</v>
-      </c>
-      <c r="E38" s="16" t="s">
-        <v>95</v>
-      </c>
-      <c r="F38" s="14" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="39" ht="14.25" customHeight="1">
-      <c r="A39" s="4" t="s">
-        <v>98</v>
-      </c>
-      <c r="B39" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C39" s="4" t="s">
-        <v>121</v>
-      </c>
-      <c r="D39" s="4"/>
-      <c r="E39" s="35">
-        <v>0.0</v>
-      </c>
-      <c r="F39" s="36">
-        <f t="shared" ref="F39:F43" si="6">D39*E39</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="40" ht="14.25" customHeight="1">
-      <c r="A40" s="4" t="s">
-        <v>101</v>
-      </c>
-      <c r="B40" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C40" s="37" t="s">
-        <v>123</v>
-      </c>
-      <c r="D40" s="4"/>
-      <c r="E40" s="35">
-        <v>0.0</v>
-      </c>
-      <c r="F40" s="36">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="41" ht="14.25" customHeight="1">
-      <c r="A41" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="B41" s="4" t="s">
-        <v>102</v>
-      </c>
-      <c r="C41" s="4" t="s">
-        <v>125</v>
-      </c>
-      <c r="D41" s="4"/>
-      <c r="E41" s="35">
-        <v>0.0</v>
-      </c>
-      <c r="F41" s="36">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="42" ht="14.25" customHeight="1">
-      <c r="A42" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="B42" s="4" t="s">
-        <v>103</v>
-      </c>
-      <c r="C42" s="4" t="s">
-        <v>126</v>
-      </c>
-      <c r="D42" s="4"/>
-      <c r="E42" s="35">
-        <v>0.0</v>
-      </c>
-      <c r="F42" s="36">
-        <f t="shared" si="6"/>
-        <v>0</v>
+      <c r="C42" s="15" t="s">
+        <v>106</v>
+      </c>
+      <c r="D42" s="13" t="s">
+        <v>129</v>
+      </c>
+      <c r="E42" s="15" t="s">
+        <v>108</v>
+      </c>
+      <c r="F42" s="13" t="s">
+        <v>149</v>
       </c>
     </row>
     <row r="43" ht="14.25" customHeight="1">
       <c r="A43" s="4" t="s">
-        <v>105</v>
+        <v>112</v>
       </c>
       <c r="B43" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="C43" s="4" t="s">
-        <v>126</v>
-      </c>
-      <c r="D43" s="4"/>
-      <c r="E43" s="35">
-        <v>0.0</v>
-      </c>
-      <c r="F43" s="36">
+        <v>6</v>
+      </c>
+      <c r="C43" s="19" t="s">
+        <v>113</v>
+      </c>
+      <c r="D43" s="19">
+        <v>10416.0</v>
+      </c>
+      <c r="E43" s="36">
+        <v>6.0</v>
+      </c>
+      <c r="F43" s="37">
+        <f t="shared" ref="F43:F48" si="6">D43*E43</f>
+        <v>62496</v>
+      </c>
+    </row>
+    <row r="44" ht="14.25" customHeight="1">
+      <c r="A44" s="4" t="s">
+        <v>120</v>
+      </c>
+      <c r="B44" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C44" s="23" t="s">
+        <v>113</v>
+      </c>
+      <c r="D44" s="19">
+        <v>7689.0</v>
+      </c>
+      <c r="E44" s="36">
+        <v>22.0</v>
+      </c>
+      <c r="F44" s="37">
         <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="44" ht="14.25" customHeight="1">
-      <c r="A44" s="4"/>
-      <c r="B44" s="6" t="s">
-        <v>129</v>
-      </c>
-      <c r="C44" s="7"/>
-      <c r="D44" s="7"/>
-      <c r="E44" s="8"/>
-      <c r="F44" s="36">
-        <f>SUM(F39:F43)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="45" ht="14.25" customHeight="1"/>
-    <row r="46" ht="14.25" customHeight="1"/>
-    <row r="47" ht="14.25" customHeight="1"/>
-    <row r="48" ht="14.25" customHeight="1"/>
-    <row r="49" ht="14.25" customHeight="1"/>
+        <v>169158</v>
+      </c>
+    </row>
+    <row r="45" ht="14.25" customHeight="1">
+      <c r="A45" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B45" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="C45" s="19" t="s">
+        <v>25</v>
+      </c>
+      <c r="D45" s="19">
+        <v>7500.0</v>
+      </c>
+      <c r="E45" s="36">
+        <v>10.0</v>
+      </c>
+      <c r="F45" s="37">
+        <f t="shared" si="6"/>
+        <v>75000</v>
+      </c>
+    </row>
+    <row r="46" ht="14.25" customHeight="1">
+      <c r="A46" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B46" s="4" t="s">
+        <v>122</v>
+      </c>
+      <c r="C46" s="19" t="s">
+        <v>123</v>
+      </c>
+      <c r="D46" s="19">
+        <v>6666.0</v>
+      </c>
+      <c r="E46" s="36">
+        <v>10.0</v>
+      </c>
+      <c r="F46" s="37">
+        <f t="shared" si="6"/>
+        <v>66660</v>
+      </c>
+    </row>
+    <row r="47" ht="14.25" customHeight="1">
+      <c r="A47" s="4" t="s">
+        <v>132</v>
+      </c>
+      <c r="B47" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C47" s="19" t="s">
+        <v>25</v>
+      </c>
+      <c r="D47" s="19">
+        <v>7852.0</v>
+      </c>
+      <c r="E47" s="36">
+        <v>6.0</v>
+      </c>
+      <c r="F47" s="37">
+        <f t="shared" si="6"/>
+        <v>47112</v>
+      </c>
+    </row>
+    <row r="48" ht="14.25" customHeight="1">
+      <c r="A48" s="19" t="s">
+        <v>133</v>
+      </c>
+      <c r="B48" s="19" t="s">
+        <v>127</v>
+      </c>
+      <c r="C48" s="19" t="s">
+        <v>123</v>
+      </c>
+      <c r="D48" s="19">
+        <v>14583.0</v>
+      </c>
+      <c r="E48" s="36">
+        <v>16.0</v>
+      </c>
+      <c r="F48" s="37">
+        <f t="shared" si="6"/>
+        <v>233328</v>
+      </c>
+    </row>
+    <row r="49" ht="14.25" customHeight="1">
+      <c r="A49" s="4"/>
+      <c r="B49" s="6" t="s">
+        <v>150</v>
+      </c>
+      <c r="C49" s="7"/>
+      <c r="D49" s="7"/>
+      <c r="E49" s="8"/>
+      <c r="F49" s="37">
+        <f>SUM(F43:F48)</f>
+        <v>653754</v>
+      </c>
+    </row>
     <row r="50" ht="14.25" customHeight="1"/>
     <row r="51" ht="14.25" customHeight="1"/>
     <row r="52" ht="14.25" customHeight="1"/>
@@ -4500,16 +4939,22 @@
     <row r="998" ht="14.25" customHeight="1"/>
     <row r="999" ht="14.25" customHeight="1"/>
     <row r="1000" ht="14.25" customHeight="1"/>
+    <row r="1001" ht="14.25" customHeight="1"/>
+    <row r="1002" ht="14.25" customHeight="1"/>
+    <row r="1003" ht="14.25" customHeight="1"/>
+    <row r="1004" ht="14.25" customHeight="1"/>
+    <row r="1005" ht="14.25" customHeight="1"/>
   </sheetData>
-  <mergeCells count="8">
+  <mergeCells count="9">
+    <mergeCell ref="B39:E39"/>
+    <mergeCell ref="B49:E49"/>
     <mergeCell ref="H2:K2"/>
-    <mergeCell ref="B8:E8"/>
-    <mergeCell ref="H11:I11"/>
-    <mergeCell ref="B17:E17"/>
-    <mergeCell ref="H20:I20"/>
-    <mergeCell ref="B26:E26"/>
-    <mergeCell ref="B35:E35"/>
-    <mergeCell ref="B44:E44"/>
+    <mergeCell ref="L2:O2"/>
+    <mergeCell ref="B9:E9"/>
+    <mergeCell ref="H12:I12"/>
+    <mergeCell ref="B19:E19"/>
+    <mergeCell ref="H22:I22"/>
+    <mergeCell ref="B29:E29"/>
   </mergeCells>
   <printOptions/>
   <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>

</xml_diff>